<commit_message>
Remove lame attempt at processing quarterly tasks.
</commit_message>
<xml_diff>
--- a/var/skuld-base.xlsx
+++ b/var/skuld-base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\J70397102-skuld\var\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{83E4D5DE-83D9-4025-BAF3-8407F0897454}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67033E88-B7F8-4D6A-984A-21D033E943EA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4590" yWindow="3915" windowWidth="23730" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="450" yWindow="2580" windowWidth="23730" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tasks" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Which Week" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tasks!$A$1:$L$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tasks!$A$1:$L$48</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="104">
   <si>
     <t>Task Name</t>
   </si>
@@ -590,7 +590,13 @@
     <t>TXCU</t>
   </si>
   <si>
-    <t>Quarterly Start</t>
+    <t>Paypal</t>
+  </si>
+  <si>
+    <t>Costco Visa 4995</t>
+  </si>
+  <si>
+    <t>Month in Quarter</t>
   </si>
 </sst>
 </file>
@@ -765,7 +771,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -943,12 +949,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1141,14 +1141,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1169,6 +1166,10 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1527,21 +1528,21 @@
   <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E52" sqref="E52"/>
+      <selection pane="bottomRight" activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="55.125" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.875" customWidth="1"/>
-    <col min="5" max="5" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.75" customWidth="1"/>
-    <col min="7" max="7" width="15.75" style="19" customWidth="1"/>
-    <col min="8" max="8" width="16.75" customWidth="1"/>
-    <col min="10" max="11" width="15.375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.75" customWidth="1"/>
+    <col min="6" max="6" width="15.75" style="16" customWidth="1"/>
+    <col min="7" max="7" width="16.75" customWidth="1"/>
+    <col min="9" max="10" width="15.375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1555,31 +1556,31 @@
         <v>5</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>101</v>
+        <v>59</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="F1" s="15" t="s">
         <v>63</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="H1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="I1" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="J1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="3" t="s">
         <v>97</v>
       </c>
+      <c r="K1" s="2" t="s">
+        <v>93</v>
+      </c>
       <c r="L1" s="2" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1592,137 +1593,155 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="E2">
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="F2" s="1">
-        <f ca="1">dates!$B$3+E2-1</f>
+      <c r="E2" s="1">
+        <f ca="1">dates!$B$3+D2-1</f>
         <v>43891</v>
       </c>
-      <c r="G2" s="19">
+      <c r="F2" s="16">
         <v>21</v>
       </c>
-      <c r="H2" s="1">
-        <f ca="1">IF(G2&gt;=E2,dates!$B$3+G2-1,dates!$B$6+G2-1)</f>
+      <c r="G2" s="1">
+        <f ca="1">IF(F2&gt;=D2,dates!$B$3+F2-1,dates!$B$6+F2-1)</f>
         <v>43911</v>
       </c>
-      <c r="I2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="1">
-        <f ca="1">NOW()</f>
-        <v>43877.752041898151</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>94</v>
+      </c>
+      <c r="K2" s="1" t="str">
+        <f>"S/S: "&amp;J2</f>
+        <v>S/S: MFCU</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="E3">
-        <v>11</v>
-      </c>
-      <c r="F3" s="1">
-        <f ca="1">dates!$B$3+E3-1</f>
-        <v>43901</v>
-      </c>
-      <c r="G3" s="19">
-        <v>11</v>
-      </c>
-      <c r="H3" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="1">
-        <f t="shared" ref="J3:J44" ca="1" si="0">NOW()</f>
-        <v>43877.752041898151</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>95</v>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3" s="1">
+        <f ca="1">dates!$B$3+D3-1</f>
+        <v>43910</v>
+      </c>
+      <c r="F3" s="16">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1">
+        <f ca="1">IF(F3&gt;=D3,dates!$B$3+F3-1,dates!$B$6+F3-1)</f>
+        <v>43938</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K3" s="1" t="str">
+        <f t="shared" ref="K3:K44" si="0">"S/S: "&amp;J3</f>
+        <v>S/S: MFCU</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="E4">
-        <v>19</v>
-      </c>
-      <c r="F4" s="1">
-        <f ca="1">dates!$B$3+E4-1</f>
-        <v>43909</v>
-      </c>
-      <c r="G4" s="19">
-        <v>19</v>
-      </c>
-      <c r="H4" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>95</v>
+      <c r="D4">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1">
+        <f ca="1">dates!$B$3+D4-1</f>
+        <v>43904</v>
+      </c>
+      <c r="F4" s="16">
+        <v>28</v>
+      </c>
+      <c r="G4" s="1">
+        <f ca="1">IF(F4&gt;=D4,dates!$B$3+F4-1,dates!$B$6+F4-1)</f>
+        <v>43918</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: MFCU</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="E5">
-        <v>20</v>
-      </c>
-      <c r="F5" s="1">
-        <f ca="1">dates!$B$3+E5-1</f>
-        <v>43910</v>
-      </c>
-      <c r="G5" s="19">
-        <v>17</v>
-      </c>
-      <c r="H5" s="1">
-        <f ca="1">IF(G5&gt;=E5,dates!$B$3+G5-1,dates!$B$6+G5-1)</f>
-        <v>43938</v>
-      </c>
-      <c r="I5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>94</v>
+      <c r="D5">
+        <v>21</v>
+      </c>
+      <c r="E5" s="1">
+        <f ca="1">dates!$B$3+D5-1</f>
+        <v>43911</v>
+      </c>
+      <c r="F5" s="16">
+        <v>25</v>
+      </c>
+      <c r="G5" s="1">
+        <f ca="1">IF(F5&gt;=D5,dates!$B$3+F5-1,dates!$B$6+F5-1)</f>
+        <v>43915</v>
+      </c>
+      <c r="H5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="K5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: BoA MC 0766</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -1730,104 +1749,116 @@
       <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="E6">
-        <v>14</v>
-      </c>
-      <c r="F6" s="1">
-        <f ca="1">dates!$B$3+E6-1</f>
-        <v>43904</v>
-      </c>
-      <c r="G6" s="19">
-        <v>28</v>
-      </c>
-      <c r="H6" s="1">
-        <f ca="1">IF(G6&gt;=E6,dates!$B$3+G6-1,dates!$B$6+G6-1)</f>
-        <v>43918</v>
-      </c>
-      <c r="I6" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-      <c r="K6" s="1" t="s">
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1">
+        <f ca="1">dates!$B$3+D6-1</f>
+        <v>43910</v>
+      </c>
+      <c r="F6" s="16">
+        <v>16</v>
+      </c>
+      <c r="G6" s="1">
+        <f ca="1">IF(F6&gt;=D6,dates!$B$3+F6-1,dates!$B$6+F6-1)</f>
+        <v>43937</v>
+      </c>
+      <c r="H6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>94</v>
+      </c>
+      <c r="K6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: MFCU</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="E7">
-        <v>21</v>
-      </c>
-      <c r="F7" s="1">
-        <f ca="1">dates!$B$3+E7-1</f>
-        <v>43911</v>
-      </c>
-      <c r="G7" s="19">
-        <v>25</v>
-      </c>
-      <c r="H7" s="1">
-        <f ca="1">IF(G7&gt;=E7,dates!$B$3+G7-1,dates!$B$6+G7-1)</f>
-        <v>43915</v>
-      </c>
-      <c r="I7" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>96</v>
+      <c r="D7">
+        <v>23</v>
+      </c>
+      <c r="E7" s="1">
+        <f ca="1">dates!$B$3+D7-1</f>
+        <v>43913</v>
+      </c>
+      <c r="F7" s="16">
+        <v>20</v>
+      </c>
+      <c r="G7" s="1">
+        <f ca="1">IF(F7&gt;=D7,dates!$B$3+F7-1,dates!$B$6+F7-1)</f>
+        <v>43941</v>
+      </c>
+      <c r="H7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: MFCU</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
-      <c r="E8">
-        <v>20</v>
-      </c>
-      <c r="F8" s="1">
-        <f ca="1">dates!$B$3+E8-1</f>
-        <v>43910</v>
-      </c>
-      <c r="G8" s="19">
-        <v>16</v>
-      </c>
-      <c r="H8" s="1">
-        <f ca="1">IF(G8&gt;=E8,dates!$B$3+G8-1,dates!$B$6+G8-1)</f>
-        <v>43937</v>
-      </c>
-      <c r="I8" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>94</v>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1">
+        <f ca="1">dates!$B$3+D8-1</f>
+        <v>43897</v>
+      </c>
+      <c r="F8" s="16">
+        <v>9</v>
+      </c>
+      <c r="G8" s="1">
+        <f ca="1">IF(F8&gt;=D8,dates!$B$3+F8-1,dates!$B$6+F8-1)</f>
+        <v>43899</v>
+      </c>
+      <c r="H8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: SSA</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -1835,58 +1866,73 @@
       <c r="C9" t="s">
         <v>10</v>
       </c>
-      <c r="E9">
+      <c r="D9">
         <v>7</v>
       </c>
-      <c r="F9" s="1">
-        <f ca="1">dates!$B$3+E9-1</f>
+      <c r="E9" s="1">
+        <f ca="1">dates!$B$3+D9-1</f>
         <v>43897</v>
       </c>
-      <c r="G9" s="19">
-        <v>9</v>
-      </c>
-      <c r="H9" s="1">
-        <f ca="1">IF(G9&gt;=E9,dates!$B$3+G9-1,dates!$B$6+G9-1)</f>
-        <v>43899</v>
-      </c>
-      <c r="I9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J9" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
+      <c r="F9" s="16">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1">
+        <f ca="1">IF(F9&gt;=D9,dates!$B$3+F9-1,dates!$B$6+F9-1)</f>
+        <v>43923</v>
+      </c>
+      <c r="H9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: SSA</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
-      <c r="E10">
+      <c r="D10">
+        <f ca="1">DAY(dates!$B$4)</f>
+        <v>31</v>
+      </c>
+      <c r="E10" s="1">
+        <f ca="1">dates!$B$4</f>
+        <v>43921</v>
+      </c>
+      <c r="F10" s="16">
         <v>7</v>
       </c>
-      <c r="F10" s="1">
-        <f ca="1">dates!$B$3+E10-1</f>
-        <v>43897</v>
-      </c>
-      <c r="G10" s="19">
-        <v>2</v>
-      </c>
-      <c r="H10" s="1">
-        <f ca="1">IF(G10&gt;=E10,dates!$B$3+G10-1,dates!$B$6+G10-1)</f>
-        <v>43923</v>
-      </c>
-      <c r="I10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J10" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
+      <c r="G10" s="1">
+        <f ca="1">IF(F10&gt;=D10,dates!$B$3+F10-1,dates!$B$6+F10-1)</f>
+        <v>43928</v>
+      </c>
+      <c r="H10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="K10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: Coastal</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1899,26 +1945,33 @@
       <c r="C11" t="s">
         <v>10</v>
       </c>
-      <c r="E11">
+      <c r="D11">
         <v>28</v>
       </c>
-      <c r="F11" s="1">
-        <f ca="1">dates!$B$3+E11-1</f>
+      <c r="E11" s="1">
+        <f ca="1">dates!$B$3+D11-1</f>
         <v>43918</v>
       </c>
-      <c r="G11" s="19">
+      <c r="F11" s="16">
         <v>23</v>
       </c>
-      <c r="H11" s="1">
-        <f ca="1">IF(G11&gt;=E11,dates!$B$3+G11-1,dates!$B$6+G11-1)</f>
+      <c r="G11" s="1">
+        <f ca="1">IF(F11&gt;=D11,dates!$B$3+F11-1,dates!$B$6+F11-1)</f>
         <v>43944</v>
       </c>
-      <c r="I11" t="s">
-        <v>9</v>
-      </c>
-      <c r="J11" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
+      <c r="H11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: MFCU</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1931,26 +1984,33 @@
       <c r="C12" t="s">
         <v>10</v>
       </c>
-      <c r="E12">
+      <c r="D12">
         <v>16</v>
       </c>
-      <c r="F12" s="1">
-        <f ca="1">dates!$B$3+E12-1</f>
+      <c r="E12" s="1">
+        <f ca="1">dates!$B$3+D12-1</f>
         <v>43906</v>
       </c>
-      <c r="G12" s="19">
+      <c r="F12" s="16">
         <v>13</v>
       </c>
-      <c r="H12" s="1">
-        <f ca="1">IF(G12&gt;=E12,dates!$B$3+G12-1,dates!$B$6+G12-1)</f>
+      <c r="G12" s="1">
+        <f ca="1">IF(F12&gt;=D12,dates!$B$3+F12-1,dates!$B$6+F12-1)</f>
         <v>43934</v>
       </c>
-      <c r="I12" t="s">
-        <v>9</v>
-      </c>
-      <c r="J12" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
+      <c r="H12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: MFCU</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1963,66 +2023,77 @@
       <c r="C13" t="s">
         <v>10</v>
       </c>
-      <c r="E13">
+      <c r="D13">
         <v>14</v>
       </c>
-      <c r="F13" s="1">
-        <f ca="1">dates!$B$3+E13-1</f>
+      <c r="E13" s="1">
+        <f ca="1">dates!$B$3+D13-1</f>
         <v>43904</v>
       </c>
-      <c r="G13" s="19">
+      <c r="F13" s="16">
         <v>7</v>
       </c>
-      <c r="H13" s="1">
-        <f ca="1">IF(G13&gt;=E13,dates!$B$3+G13-1,dates!$B$6+G13-1)</f>
+      <c r="G13" s="1">
+        <f ca="1">IF(F13&gt;=D13,dates!$B$3+F13-1,dates!$B$6+F13-1)</f>
         <v>43928</v>
       </c>
-      <c r="I13" t="s">
-        <v>9</v>
-      </c>
-      <c r="J13" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
+      <c r="H13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: MFCU</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
       </c>
-      <c r="E14">
-        <v>28</v>
-      </c>
-      <c r="F14" s="1">
-        <f ca="1">dates!$B$3+E14-1</f>
-        <v>43918</v>
-      </c>
-      <c r="G14" s="19">
-        <v>28</v>
-      </c>
-      <c r="H14" s="1">
-        <f ca="1">IF(G14&gt;=E14,dates!$B$3+G14-1,dates!$B$6+G14-1)</f>
-        <v>43918</v>
-      </c>
-      <c r="I14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J14" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-      <c r="K14" s="1" t="s">
+      <c r="D14">
+        <v>17</v>
+      </c>
+      <c r="E14" s="1">
+        <f ca="1">dates!$B$3+D14-1</f>
+        <v>43907</v>
+      </c>
+      <c r="F14" s="16">
+        <v>10</v>
+      </c>
+      <c r="G14" s="1">
+        <f ca="1">IF(F14&gt;=D14,dates!$B$3+F14-1,dates!$B$6+F14-1)</f>
+        <v>43931</v>
+      </c>
+      <c r="H14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>94</v>
+      </c>
+      <c r="K14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: MFCU</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
         <v>23</v>
@@ -2030,925 +2101,1062 @@
       <c r="C15" t="s">
         <v>10</v>
       </c>
-      <c r="E15">
+      <c r="D15">
         <v>28</v>
       </c>
-      <c r="F15" s="1">
-        <f ca="1">dates!$B$3+E15-1</f>
+      <c r="E15" s="1">
+        <f ca="1">dates!$B$3+D15-1</f>
         <v>43918</v>
       </c>
-      <c r="G15" s="19">
+      <c r="F15" s="16">
         <v>28</v>
       </c>
-      <c r="H15" s="1">
-        <f ca="1">IF(G15&gt;=E15,dates!$B$3+G15-1,dates!$B$6+G15-1)</f>
+      <c r="G15" s="1">
+        <f ca="1">IF(F15&gt;=D15,dates!$B$3+F15-1,dates!$B$6+F15-1)</f>
         <v>43918</v>
       </c>
-      <c r="I15" t="s">
-        <v>9</v>
-      </c>
-      <c r="J15" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-      <c r="K15" s="1" t="s">
+      <c r="H15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>94</v>
+      </c>
+      <c r="K15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: MFCU</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>28</v>
+      </c>
+      <c r="E16" s="1">
+        <f ca="1">dates!$B$3+D16-1</f>
+        <v>43918</v>
+      </c>
+      <c r="F16" s="16">
+        <v>28</v>
+      </c>
+      <c r="G16" s="1">
+        <f ca="1">IF(F16&gt;=D16,dates!$B$3+F16-1,dates!$B$6+F16-1)</f>
+        <v>43918</v>
+      </c>
+      <c r="H16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: MFCU</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>8</v>
       </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16">
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17">
         <v>26</v>
       </c>
-      <c r="F16" s="1">
-        <f ca="1">dates!$B$3+E16-1</f>
+      <c r="E17" s="1">
+        <f ca="1">dates!$B$3+D17-1</f>
         <v>43916</v>
       </c>
-      <c r="G16" s="19">
+      <c r="F17" s="16">
         <v>21</v>
       </c>
-      <c r="H16" s="1">
-        <f ca="1">IF(G16&gt;=E16,dates!$B$3+G16-1,dates!$B$6+G16-1)</f>
+      <c r="G17" s="1">
+        <f ca="1">IF(F17&gt;=D17,dates!$B$3+F17-1,dates!$B$6+F17-1)</f>
         <v>43942</v>
       </c>
-      <c r="I16" t="s">
-        <v>9</v>
-      </c>
-      <c r="J16" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="H17" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: MFCU</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>60</v>
       </c>
-      <c r="C17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17">
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18">
         <v>8</v>
       </c>
-      <c r="F17" s="1">
-        <f ca="1">dates!$B$3+E17-1</f>
+      <c r="E18" s="1">
+        <f ca="1">dates!$B$3+D18-1</f>
         <v>43898</v>
       </c>
-      <c r="G17" s="19">
+      <c r="F18" s="16">
         <v>19</v>
       </c>
-      <c r="H17" s="1">
-        <f ca="1">IF(G17&gt;=E17,dates!$B$3+G17-1,dates!$B$6+G17-1)</f>
+      <c r="G18" s="1">
+        <f ca="1">IF(F18&gt;=D18,dates!$B$3+F18-1,dates!$B$6+F18-1)</f>
         <v>43909</v>
       </c>
-      <c r="I17" t="s">
-        <v>9</v>
-      </c>
-      <c r="J17" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-      <c r="K17" s="1" t="s">
+      <c r="H18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J18" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="K18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: BoA MC 0766</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>61</v>
       </c>
-      <c r="C18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18">
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19">
         <v>8</v>
       </c>
-      <c r="F18" s="1">
-        <f ca="1">dates!$B$3+E18-1</f>
+      <c r="E19" s="1">
+        <f ca="1">dates!$B$3+D19-1</f>
         <v>43898</v>
       </c>
-      <c r="G18" s="19">
+      <c r="F19" s="16">
         <v>8</v>
       </c>
-      <c r="H18" s="1">
-        <f ca="1">IF(G18&gt;=E18,dates!$B$3+G18-1,dates!$B$6+G18-1)</f>
+      <c r="G19" s="1">
+        <f ca="1">IF(F19&gt;=D19,dates!$B$3+F19-1,dates!$B$6+F19-1)</f>
         <v>43898</v>
       </c>
-      <c r="I18" t="s">
-        <v>9</v>
-      </c>
-      <c r="J18" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-      <c r="K18" s="1" t="s">
+      <c r="H19" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J19" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="K19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: BoA MC 0766</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>8</v>
       </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19">
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20">
         <v>17</v>
       </c>
-      <c r="F19" s="1">
-        <f ca="1">dates!$B$3+E19-1</f>
+      <c r="E20" s="1">
+        <f ca="1">dates!$B$3+D20-1</f>
         <v>43907</v>
       </c>
-      <c r="G19" s="19">
+      <c r="F20" s="16">
         <v>13</v>
       </c>
-      <c r="H19" s="1">
-        <f ca="1">IF(G19&gt;=E19,dates!$B$3+G19-1,dates!$B$6+G19-1)</f>
+      <c r="G20" s="1">
+        <f ca="1">IF(F20&gt;=D20,dates!$B$3+F20-1,dates!$B$6+F20-1)</f>
         <v>43934</v>
       </c>
-      <c r="I19" t="s">
-        <v>9</v>
-      </c>
-      <c r="J19" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="H20" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: MFCU</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>61</v>
       </c>
-      <c r="C20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20">
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21">
         <v>11</v>
       </c>
-      <c r="F20" s="1">
-        <f ca="1">dates!$B$3+E20-1</f>
+      <c r="E21" s="1">
+        <f ca="1">dates!$B$3+D21-1</f>
         <v>43901</v>
       </c>
-      <c r="G20" s="19">
-        <v>10</v>
-      </c>
-      <c r="H20" s="1">
-        <f ca="1">IF(G20&gt;=E20,dates!$B$3+G20-1,dates!$B$6+G20-1)</f>
+      <c r="F21" s="16">
+        <v>10</v>
+      </c>
+      <c r="G21" s="1">
+        <f ca="1">IF(F21&gt;=D21,dates!$B$3+F21-1,dates!$B$6+F21-1)</f>
         <v>43931</v>
       </c>
-      <c r="I20" t="s">
-        <v>9</v>
-      </c>
-      <c r="J20" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="H21" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="K21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: Paypal</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21">
+      <c r="C22" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="19">
         <f ca="1">DAY(dates!$B$4)</f>
         <v>31</v>
       </c>
-      <c r="F21" s="1">
+      <c r="E22" s="20">
         <f ca="1">dates!$B$4</f>
         <v>43921</v>
       </c>
-      <c r="G21" s="19">
+      <c r="F22" s="21">
         <v>7</v>
       </c>
-      <c r="H21" s="1">
-        <f ca="1">dates!B4</f>
-        <v>43921</v>
-      </c>
-      <c r="I21" t="s">
-        <v>9</v>
-      </c>
-      <c r="J21" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-      <c r="K21" s="1" t="s">
+      <c r="G22" s="20">
+        <f ca="1">E22+7</f>
+        <v>43928</v>
+      </c>
+      <c r="H22" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="I22" s="20">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J22" s="20" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="K22" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: MFCU</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="19">
+        <v>1</v>
+      </c>
+      <c r="E23" s="20">
+        <f ca="1">dates!$B$3+D23-1</f>
+        <v>43891</v>
+      </c>
+      <c r="F23" s="21">
+        <v>20</v>
+      </c>
+      <c r="G23" s="20">
+        <f ca="1">IF(F23&gt;=D23,dates!$B$3+F23-1,dates!$B$6+F23-1)</f>
+        <v>43910</v>
+      </c>
+      <c r="H23" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="I23" s="20">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J23" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="K23" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: SSA</v>
+      </c>
+      <c r="L23" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B24" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C24" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="E22">
-        <v>29</v>
-      </c>
-      <c r="F22" s="1">
-        <f ca="1">dates!$B$3+E22-1</f>
-        <v>43919</v>
-      </c>
-      <c r="G22" s="19">
+      <c r="D24" s="19">
+        <v>1</v>
+      </c>
+      <c r="E24" s="20">
+        <f ca="1">dates!$B$3+D24-1</f>
+        <v>43891</v>
+      </c>
+      <c r="F24" s="21">
         <v>20</v>
       </c>
-      <c r="H22" s="1">
-        <f ca="1">IF(G22&gt;=E22,dates!$B$3+G22-1,dates!$B$6+G22-1)</f>
-        <v>43941</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J22" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-      <c r="K22" s="6" t="s">
+      <c r="G24" s="20">
+        <f ca="1">IF(F24&gt;=D24,dates!$B$3+F24-1,dates!$B$6+F24-1)</f>
+        <v>43910</v>
+      </c>
+      <c r="H24" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="I24" s="20">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J24" s="20" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B23" s="5" t="s">
+      <c r="K24" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: SSA</v>
+      </c>
+      <c r="L24" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23">
-        <v>29</v>
-      </c>
-      <c r="F23" s="1">
-        <f ca="1">dates!$B$3+E23-1</f>
-        <v>43919</v>
-      </c>
-      <c r="G23" s="19">
+      <c r="C25" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="19">
+        <v>1</v>
+      </c>
+      <c r="E25" s="20">
+        <f ca="1">dates!$B$3+D25-1</f>
+        <v>43891</v>
+      </c>
+      <c r="F25" s="21">
         <v>20</v>
       </c>
-      <c r="H23" s="1">
-        <f ca="1">IF(G23&gt;=E23,dates!$B$3+G23-1,dates!$B$6+G23-1)</f>
-        <v>43941</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J23" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-      <c r="K23" s="6" t="s">
+      <c r="G25" s="20">
+        <f ca="1">IF(F25&gt;=D25,dates!$B$3+F25-1,dates!$B$6+F25-1)</f>
+        <v>43910</v>
+      </c>
+      <c r="H25" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="I25" s="20">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J25" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="K25" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: MFCU</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26">
+        <v>17</v>
+      </c>
+      <c r="E26" s="1">
+        <f ca="1">dates!$B$3+D26-1</f>
+        <v>43907</v>
+      </c>
+      <c r="F26" s="16">
+        <v>17</v>
+      </c>
+      <c r="G26" s="1">
+        <f ca="1">IF(F26&gt;=D26,dates!$B$3+F26-1,dates!$B$6+F26-1)</f>
+        <v>43907</v>
+      </c>
+      <c r="H26" t="s">
+        <v>9</v>
+      </c>
+      <c r="I26" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: Costco Visa 4995</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1">
+        <f ca="1">dates!$B$3+D27-1</f>
+        <v>43891</v>
+      </c>
+      <c r="F27" s="16">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1">
+        <f ca="1">IF(F27&gt;=D27,dates!$B$3+F27-1,dates!$B$6+F27-1)</f>
+        <v>43891</v>
+      </c>
+      <c r="H27" t="s">
+        <v>9</v>
+      </c>
+      <c r="I27" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="K27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: BoA MC 0766</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28">
+        <v>20</v>
+      </c>
+      <c r="E28" s="1">
+        <f ca="1">dates!$B$3+D28-1</f>
+        <v>43910</v>
+      </c>
+      <c r="F28" s="16">
+        <v>17</v>
+      </c>
+      <c r="G28" s="1">
+        <f ca="1">IF(F28&gt;=D28,dates!$B$3+F28-1,dates!$B$6+F28-1)</f>
+        <v>43938</v>
+      </c>
+      <c r="H28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I28" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: MFCU</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29">
+        <v>11</v>
+      </c>
+      <c r="E29" s="1">
+        <f ca="1">dates!$B$3+D29-1</f>
+        <v>43901</v>
+      </c>
+      <c r="F29" s="16">
+        <v>11</v>
+      </c>
+      <c r="G29" s="1">
+        <f ca="1">IF(F29&gt;=D29,dates!$B$3+F29-1,dates!$B$6+F29-1)</f>
+        <v>43901</v>
+      </c>
+      <c r="H29" t="s">
+        <v>9</v>
+      </c>
+      <c r="I29" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J29" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="F24" s="1">
-        <f ca="1">dates!$B$3+E24-1</f>
-        <v>43891</v>
-      </c>
-      <c r="G24" s="19">
-        <v>1</v>
-      </c>
-      <c r="H24" s="1">
-        <f ca="1">IF(G24&gt;=E24,dates!$B$3+G24-1,dates!$B$6+G24-1)</f>
-        <v>43891</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J24" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-      <c r="K24" s="6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25">
-        <v>17</v>
-      </c>
-      <c r="F25" s="1">
-        <f ca="1">dates!$B$3+E25-1</f>
-        <v>43907</v>
-      </c>
-      <c r="G25" s="19">
-        <v>17</v>
-      </c>
-      <c r="H25" s="1">
-        <f ca="1">IF(G25&gt;=E25,dates!$B$3+G25-1,dates!$B$6+G25-1)</f>
-        <v>43907</v>
-      </c>
-      <c r="I25" t="s">
-        <v>9</v>
-      </c>
-      <c r="J25" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26" s="1">
-        <f ca="1">dates!$B$3+E26-1</f>
-        <v>43891</v>
-      </c>
-      <c r="G26" s="19">
-        <v>1</v>
-      </c>
-      <c r="H26" s="1">
-        <f ca="1">IF(G26&gt;=E26,dates!$B$3+G26-1,dates!$B$6+G26-1)</f>
-        <v>43891</v>
-      </c>
-      <c r="I26" t="s">
-        <v>9</v>
-      </c>
-      <c r="J26" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-      <c r="K26" s="1" t="s">
+      <c r="K29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: SSA</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30">
+        <v>15</v>
+      </c>
+      <c r="E30" s="1">
+        <f ca="1">dates!$B$3+D30-1</f>
+        <v>43905</v>
+      </c>
+      <c r="F30" s="16">
+        <v>18</v>
+      </c>
+      <c r="G30" s="1">
+        <f ca="1">IF(F30&gt;=D30,dates!$B$3+F30-1,dates!$B$6+F30-1)</f>
+        <v>43908</v>
+      </c>
+      <c r="H30" t="s">
+        <v>9</v>
+      </c>
+      <c r="I30" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: SSA</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31">
+        <v>15</v>
+      </c>
+      <c r="E31" s="1">
+        <f ca="1">dates!$B$3+D31-1</f>
+        <v>43905</v>
+      </c>
+      <c r="F31" s="16">
+        <v>18</v>
+      </c>
+      <c r="G31" s="1">
+        <f ca="1">IF(F31&gt;=D31,dates!$B$3+F31-1,dates!$B$6+F31-1)</f>
+        <v>43908</v>
+      </c>
+      <c r="H31" t="s">
+        <v>9</v>
+      </c>
+      <c r="I31" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: SSA</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32">
+        <v>19</v>
+      </c>
+      <c r="E32" s="1">
+        <f ca="1">dates!$B$3+D32-1</f>
+        <v>43909</v>
+      </c>
+      <c r="F32" s="16">
+        <v>19</v>
+      </c>
+      <c r="G32" s="1">
+        <f ca="1">IF(F32&gt;=D32,dates!$B$3+F32-1,dates!$B$6+F32-1)</f>
+        <v>43909</v>
+      </c>
+      <c r="H32" t="s">
+        <v>9</v>
+      </c>
+      <c r="I32" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J32" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27">
-        <v>20</v>
-      </c>
-      <c r="F27" s="1">
-        <f ca="1">dates!$B$3+E27-1</f>
-        <v>43910</v>
-      </c>
-      <c r="G27" s="19">
-        <v>17</v>
-      </c>
-      <c r="H27" s="1">
-        <f ca="1">IF(G27&gt;=E27,dates!$B$3+G27-1,dates!$B$6+G27-1)</f>
-        <v>43938</v>
-      </c>
-      <c r="I27" t="s">
-        <v>9</v>
-      </c>
-      <c r="J27" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28">
-        <v>15</v>
-      </c>
-      <c r="F28" s="1">
-        <f ca="1">dates!$B$3+E28-1</f>
-        <v>43905</v>
-      </c>
-      <c r="G28" s="19">
-        <v>18</v>
-      </c>
-      <c r="H28" s="1">
-        <f ca="1">IF(G28&gt;=E28,dates!$B$3+G28-1,dates!$B$6+G28-1)</f>
-        <v>43908</v>
-      </c>
-      <c r="I28" t="s">
-        <v>9</v>
-      </c>
-      <c r="J28" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29">
-        <v>15</v>
-      </c>
-      <c r="F29" s="1">
-        <f ca="1">dates!$B$3+E29-1</f>
-        <v>43905</v>
-      </c>
-      <c r="G29" s="19">
-        <v>18</v>
-      </c>
-      <c r="H29" s="1">
-        <f ca="1">IF(G29&gt;=E29,dates!$B$3+G29-1,dates!$B$6+G29-1)</f>
-        <v>43908</v>
-      </c>
-      <c r="I29" t="s">
-        <v>9</v>
-      </c>
-      <c r="J29" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30">
-        <v>19</v>
-      </c>
-      <c r="F30" s="1">
-        <f ca="1">dates!$B$3+E30-1</f>
-        <v>43909</v>
-      </c>
-      <c r="G30" s="19">
-        <v>19</v>
-      </c>
-      <c r="H30" s="1">
-        <f ca="1">IF(G30&gt;=E30,dates!$B$3+G30-1,dates!$B$6+G30-1)</f>
-        <v>43909</v>
-      </c>
-      <c r="I30" t="s">
-        <v>9</v>
-      </c>
-      <c r="J30" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31">
-        <v>15</v>
-      </c>
-      <c r="F31" s="1">
-        <f ca="1">dates!$B$3+E31-1</f>
-        <v>43905</v>
-      </c>
-      <c r="G31" s="19">
-        <v>15</v>
-      </c>
-      <c r="H31" s="1">
-        <f ca="1">IF(G31&gt;=E31,dates!$B$3+G31-1,dates!$B$6+G31-1)</f>
-        <v>43905</v>
-      </c>
-      <c r="I31" t="s">
-        <v>9</v>
-      </c>
-      <c r="J31" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" t="s">
-        <v>43</v>
-      </c>
-      <c r="C32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32">
-        <v>15</v>
-      </c>
-      <c r="F32" s="1">
-        <f ca="1">dates!$B$3+E32-1</f>
-        <v>43905</v>
-      </c>
-      <c r="G32" s="19">
-        <v>15</v>
-      </c>
-      <c r="H32" s="1">
-        <f ca="1">IF(G32&gt;=E32,dates!$B$3+G32-1,dates!$B$6+G32-1)</f>
-        <v>43905</v>
-      </c>
-      <c r="I32" t="s">
-        <v>9</v>
-      </c>
-      <c r="J32" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>94</v>
+      <c r="K32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: BoA MC 0766</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33">
+        <v>5</v>
+      </c>
+      <c r="E33" s="1">
+        <f ca="1">dates!$B$3+D33-1</f>
+        <v>43895</v>
+      </c>
+      <c r="F33" s="16">
+        <v>5</v>
+      </c>
+      <c r="G33" s="1">
+        <f ca="1">IF(F33&gt;=D33,dates!$B$3+F33-1,dates!$B$6+F33-1)</f>
+        <v>43895</v>
+      </c>
+      <c r="H33" t="s">
+        <v>9</v>
+      </c>
+      <c r="I33" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: MFCU</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1">
+        <f ca="1">dates!$B$3+D34-1</f>
+        <v>43891</v>
+      </c>
+      <c r="F34" s="16">
+        <v>1</v>
+      </c>
+      <c r="G34" s="1">
+        <f ca="1">IF(F34&gt;=D34,dates!$B$3+F34-1,dates!$B$6+F34-1)</f>
+        <v>43891</v>
+      </c>
+      <c r="H34" t="s">
+        <v>9</v>
+      </c>
+      <c r="I34" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: MFCU</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1">
+        <f ca="1">dates!$B$3+D35-1</f>
+        <v>43891</v>
+      </c>
+      <c r="F35" s="16">
+        <v>6</v>
+      </c>
+      <c r="G35" s="1">
+        <f ca="1">IF(F35&gt;=D35,dates!$B$3+F35-1,dates!$B$6+F35-1)</f>
+        <v>43896</v>
+      </c>
+      <c r="H35" t="s">
+        <v>9</v>
+      </c>
+      <c r="I35" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: MFCU</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36">
+        <v>15</v>
+      </c>
+      <c r="E36" s="1">
+        <f ca="1">dates!$B$3+D36-1</f>
+        <v>43905</v>
+      </c>
+      <c r="F36" s="16">
+        <v>15</v>
+      </c>
+      <c r="G36" s="1">
+        <f ca="1">IF(F36&gt;=D36,dates!$B$3+F36-1,dates!$B$6+F36-1)</f>
+        <v>43905</v>
+      </c>
+      <c r="H36" t="s">
+        <v>9</v>
+      </c>
+      <c r="I36" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: MFCU</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37">
+        <v>15</v>
+      </c>
+      <c r="E37" s="1">
+        <f ca="1">dates!$B$3+D37-1</f>
+        <v>43905</v>
+      </c>
+      <c r="F37" s="16">
+        <v>15</v>
+      </c>
+      <c r="G37" s="1">
+        <f ca="1">IF(F37&gt;=D37,dates!$B$3+F37-1,dates!$B$6+F37-1)</f>
+        <v>43905</v>
+      </c>
+      <c r="H37" t="s">
+        <v>9</v>
+      </c>
+      <c r="I37" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: MFCU</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B38" t="s">
         <v>31</v>
       </c>
-      <c r="C33" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33">
+      <c r="C38" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38">
         <f ca="1">DAY(dates!$B$4)</f>
         <v>31</v>
       </c>
-      <c r="F33" s="1">
+      <c r="E38" s="1">
         <f ca="1">dates!$B$4</f>
         <v>43921</v>
       </c>
-      <c r="G33" s="19">
+      <c r="F38" s="16">
         <v>7</v>
       </c>
-      <c r="H33" s="1">
-        <f ca="1">IF(G33&gt;=E33,dates!$B$3+G33-1,dates!$B$6+G33-1)</f>
+      <c r="G38" s="20">
+        <f ca="1">E38+7</f>
         <v>43928</v>
       </c>
-      <c r="I33" t="s">
-        <v>9</v>
-      </c>
-      <c r="J33" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-      <c r="K33" s="1" t="s">
+      <c r="H38" t="s">
+        <v>9</v>
+      </c>
+      <c r="I38" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J38" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="K38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: TXCU</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B39" t="s">
         <v>11</v>
       </c>
-      <c r="C34" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34">
+      <c r="C39" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39">
         <v>8</v>
       </c>
-      <c r="F34" s="1">
-        <f ca="1">dates!$B$3+E34-1</f>
+      <c r="E39" s="1">
+        <f ca="1">dates!$B$3+D39-1</f>
         <v>43898</v>
       </c>
-      <c r="G34" s="19">
+      <c r="F39" s="16">
         <v>8</v>
       </c>
-      <c r="H34" s="1">
-        <f ca="1">IF(G34&gt;=E34,dates!$B$3+G34-1,dates!$B$6+G34-1)</f>
+      <c r="G39" s="1">
+        <f ca="1">IF(F39&gt;=D39,dates!$B$3+F39-1,dates!$B$6+F39-1)</f>
         <v>43898</v>
       </c>
-      <c r="I34" t="s">
-        <v>9</v>
-      </c>
-      <c r="J34" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-      <c r="K34" s="1" t="s">
+      <c r="H39" t="s">
+        <v>9</v>
+      </c>
+      <c r="I39" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J39" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="K39" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: BoA MC 0766</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B40" t="s">
         <v>31</v>
       </c>
-      <c r="C35" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35">
+      <c r="C40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40">
         <v>16</v>
       </c>
-      <c r="F35" s="1">
-        <f ca="1">dates!$B$3+E35-1</f>
+      <c r="E40" s="1">
+        <f ca="1">dates!$B$3+D40-1</f>
         <v>43906</v>
       </c>
-      <c r="G35" s="19">
-        <f>E35+7</f>
+      <c r="F40" s="16">
+        <f>D40+7</f>
         <v>23</v>
       </c>
-      <c r="H35" s="1">
-        <f ca="1">IF(G35&gt;=E35,dates!$B$3+G35-1,dates!$B$6+G35-1)</f>
+      <c r="G40" s="20">
+        <f ca="1">E40+7</f>
         <v>43913</v>
       </c>
-      <c r="I35" t="s">
-        <v>9</v>
-      </c>
-      <c r="J35" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-      <c r="K35" s="1" t="s">
+      <c r="H40" t="s">
+        <v>9</v>
+      </c>
+      <c r="I40" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J40" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="K40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: USAA</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B41" t="s">
         <v>31</v>
       </c>
-      <c r="C36" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36">
+      <c r="C41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41">
         <f ca="1">DAY(dates!$B$4)</f>
         <v>31</v>
       </c>
-      <c r="F36" s="1">
+      <c r="E41" s="1">
         <f ca="1">dates!$B$4</f>
         <v>43921</v>
       </c>
-      <c r="G36" s="19">
+      <c r="F41" s="16">
         <v>7</v>
       </c>
-      <c r="H36" s="1">
-        <f ca="1">IF(G36&gt;=E36,dates!$B$3+G36-1,dates!$B$6+G36-1)</f>
+      <c r="G41" s="20">
+        <f ca="1">dates!$B$4+7</f>
         <v>43928</v>
       </c>
-      <c r="I36" t="s">
-        <v>9</v>
-      </c>
-      <c r="J36" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-      <c r="K36" s="1" t="s">
+      <c r="H41" t="s">
+        <v>9</v>
+      </c>
+      <c r="I41" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J41" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37">
-        <v>28</v>
-      </c>
-      <c r="F37" s="1">
-        <f ca="1">dates!$B$3+E37-1</f>
-        <v>43918</v>
-      </c>
-      <c r="G37" s="19">
-        <v>28</v>
-      </c>
-      <c r="H37" s="1">
-        <f ca="1">IF(G37&gt;=E37,dates!$B$3+G37-1,dates!$B$6+G37-1)</f>
-        <v>43918</v>
-      </c>
-      <c r="I37" t="s">
-        <v>9</v>
-      </c>
-      <c r="J37" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-      <c r="K37" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B38" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38">
-        <v>15</v>
-      </c>
-      <c r="F38" s="1">
-        <f ca="1">dates!$B$3+E38-1</f>
-        <v>43905</v>
-      </c>
-      <c r="G38" s="19">
-        <v>11</v>
-      </c>
-      <c r="H38" s="1">
-        <f ca="1">IF(G38&gt;=E38,dates!$B$3+G38-1,dates!$B$6+G38-1)</f>
-        <v>43932</v>
-      </c>
-      <c r="I38" t="s">
-        <v>9</v>
-      </c>
-      <c r="J38" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B39" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39">
-        <v>23</v>
-      </c>
-      <c r="F39" s="1">
-        <f ca="1">dates!$B$3+E39-1</f>
-        <v>43913</v>
-      </c>
-      <c r="G39" s="19">
-        <v>20</v>
-      </c>
-      <c r="H39" s="1">
-        <f ca="1">IF(G39&gt;=E39,dates!$B$3+G39-1,dates!$B$6+G39-1)</f>
-        <v>43941</v>
-      </c>
-      <c r="I39" t="s">
-        <v>9</v>
-      </c>
-      <c r="J39" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B40" t="s">
-        <v>31</v>
-      </c>
-      <c r="C40" t="s">
-        <v>10</v>
-      </c>
-      <c r="E40">
-        <f ca="1">DAY(dates!$B$4)</f>
-        <v>31</v>
-      </c>
-      <c r="F40" s="1">
-        <f ca="1">dates!$B$4</f>
-        <v>43921</v>
-      </c>
-      <c r="G40" s="19">
-        <v>7</v>
-      </c>
-      <c r="H40" s="1">
-        <f ca="1">IF(G40&gt;=E40,dates!$B$3+G40-1,dates!$B$6+G40-1)</f>
-        <v>43928</v>
-      </c>
-      <c r="I40" t="s">
-        <v>9</v>
-      </c>
-      <c r="J40" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B41" t="s">
-        <v>60</v>
-      </c>
-      <c r="C41" t="s">
-        <v>10</v>
-      </c>
-      <c r="E41">
-        <v>17</v>
-      </c>
-      <c r="F41" s="1">
-        <f ca="1">dates!$B$3+E41-1</f>
-        <v>43907</v>
-      </c>
-      <c r="G41" s="19">
-        <v>10</v>
-      </c>
-      <c r="H41" s="1">
-        <f ca="1">IF(G41&gt;=E41,dates!$B$3+G41-1,dates!$B$6+G41-1)</f>
-        <v>43931</v>
-      </c>
-      <c r="I41" t="s">
-        <v>9</v>
-      </c>
-      <c r="J41" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-      <c r="K41" s="1" t="s">
-        <v>94</v>
+      <c r="K41" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: USAA</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B42" t="s">
         <v>11</v>
@@ -2956,115 +3164,131 @@
       <c r="C42" t="s">
         <v>10</v>
       </c>
-      <c r="E42">
-        <v>5</v>
-      </c>
-      <c r="F42" s="1">
-        <f ca="1">dates!$B$3+E42-1</f>
-        <v>43895</v>
-      </c>
-      <c r="G42" s="19">
-        <v>5</v>
-      </c>
-      <c r="H42" s="1">
-        <f ca="1">IF(G42&gt;=E42,dates!$B$3+G42-1,dates!$B$6+G42-1)</f>
-        <v>43895</v>
-      </c>
-      <c r="I42" t="s">
-        <v>9</v>
-      </c>
-      <c r="J42" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>94</v>
+      <c r="D42">
+        <v>28</v>
+      </c>
+      <c r="E42" s="1">
+        <f ca="1">dates!$B$3+D42-1</f>
+        <v>43918</v>
+      </c>
+      <c r="F42" s="16">
+        <v>28</v>
+      </c>
+      <c r="G42" s="1">
+        <f ca="1">IF(F42&gt;=D42,dates!$B$3+F42-1,dates!$B$6+F42-1)</f>
+        <v>43918</v>
+      </c>
+      <c r="H42" t="s">
+        <v>9</v>
+      </c>
+      <c r="I42" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K42" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: SSA</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B43" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="C43" t="s">
         <v>10</v>
       </c>
-      <c r="E43">
-        <v>1</v>
-      </c>
-      <c r="F43" s="1">
-        <f ca="1">dates!$B$3+E43-1</f>
-        <v>43891</v>
-      </c>
-      <c r="G43" s="19">
-        <v>1</v>
-      </c>
-      <c r="H43" s="1">
-        <f ca="1">IF(G43&gt;=E43,dates!$B$3+G43-1,dates!$B$6+G43-1)</f>
-        <v>43891</v>
-      </c>
-      <c r="I43" t="s">
-        <v>9</v>
-      </c>
-      <c r="J43" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-      <c r="K43" s="1" t="s">
+      <c r="D43">
+        <v>15</v>
+      </c>
+      <c r="E43" s="1">
+        <f ca="1">dates!$B$3+D43-1</f>
+        <v>43905</v>
+      </c>
+      <c r="F43" s="16">
+        <v>11</v>
+      </c>
+      <c r="G43" s="1">
+        <f ca="1">IF(F43&gt;=D43,dates!$B$3+F43-1,dates!$B$6+F43-1)</f>
+        <v>43932</v>
+      </c>
+      <c r="H43" t="s">
+        <v>9</v>
+      </c>
+      <c r="I43" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J43" s="1" t="s">
         <v>94</v>
+      </c>
+      <c r="K43" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: MFCU</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B44" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C44" t="s">
         <v>10</v>
       </c>
-      <c r="E44">
-        <v>1</v>
-      </c>
-      <c r="F44" s="1">
-        <f ca="1">dates!$B$3+E44-1</f>
-        <v>43891</v>
-      </c>
-      <c r="G44" s="19">
-        <v>6</v>
-      </c>
-      <c r="H44" s="1">
-        <f ca="1">IF(G44&gt;=E44,dates!$B$3+G44-1,dates!$B$6+G44-1)</f>
-        <v>43896</v>
-      </c>
-      <c r="I44" t="s">
-        <v>9</v>
-      </c>
-      <c r="J44" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43877.752041898151</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>94</v>
+      <c r="D44">
+        <v>19</v>
+      </c>
+      <c r="E44" s="1">
+        <f ca="1">dates!$B$3+D44-1</f>
+        <v>43909</v>
+      </c>
+      <c r="F44" s="16">
+        <f>D44</f>
+        <v>19</v>
+      </c>
+      <c r="G44" s="1">
+        <f ca="1">IF(F44&gt;=D44,dates!$B$3+F44-1,dates!$B$6+F44-1)</f>
+        <v>43909</v>
+      </c>
+      <c r="H44" t="s">
+        <v>9</v>
+      </c>
+      <c r="I44" s="1">
+        <f ca="1">NOW()</f>
+        <v>43879.431868634259</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K44" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S/S: SSA</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F45" s="1"/>
+      <c r="E45" s="1"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F46" s="1"/>
+      <c r="E46" s="1"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F47" s="1"/>
+      <c r="E47" s="1"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F48" s="1"/>
+      <c r="E48" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L49" xr:uid="{7CCF7F70-DDD4-4E75-90B0-743CA03FB5E7}"/>
+  <autoFilter ref="A1:L48" xr:uid="{88344675-4FC4-4D7C-8A53-75F0696BC5D6}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K49">
+    <sortCondition ref="A2:A49"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3102,7 +3326,7 @@
       </c>
       <c r="B2" s="1">
         <f ca="1">NOW()</f>
-        <v>43877.752041898151</v>
+        <v>43879.431868634259</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3319,6 +3543,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3331,6 +3556,7 @@
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3349,38 +3575,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="17"/>
     </row>
     <row r="2" spans="1:2" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
-      <c r="B2" s="10"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="7"/>
     </row>
     <row r="3" spans="1:2" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
     </row>
     <row r="4" spans="1:2" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="13"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="10"/>
     </row>
     <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="13" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
     </row>
     <row r="7" spans="1:2" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -3439,12 +3665,12 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
-      <c r="B15" s="10"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="7"/>
     </row>
     <row r="16" spans="1:2" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
-      <c r="B16" s="12"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
     </row>
     <row r="17" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -3452,6 +3678,7 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3474,42 +3701,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:6" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
-      <c r="B2" s="10"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="7"/>
     </row>
     <row r="3" spans="1:6" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
     </row>
     <row r="4" spans="1:6" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="13"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="10"/>
     </row>
     <row r="5" spans="1:6" s="2" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="13" t="s">
         <v>79</v>
       </c>
       <c r="D5"/>
       <c r="F5"/>
     </row>
     <row r="6" spans="1:6" s="2" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
       <c r="D6"/>
       <c r="F6"/>
     </row>
     <row r="7" spans="1:6" s="2" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
       <c r="D7"/>
       <c r="F7"/>
     </row>
@@ -3558,18 +3785,19 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-      <c r="B13" s="10"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="7"/>
     </row>
     <row r="14" spans="1:6" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="12"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="9"/>
     </row>
     <row r="15" spans="1:6" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="13"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed #36 Set Coastal Visa Download to Day 3.
</commit_message>
<xml_diff>
--- a/var/skuld-base.xlsx
+++ b/var/skuld-base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\J70397102-skuld\var\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6138F0BA-C996-4327-B4BF-392075EFF99B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB710BC-27BB-4937-AEB4-8C84CC1503E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="120" windowWidth="21000" windowHeight="13530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1260" yWindow="1650" windowWidth="21000" windowHeight="13530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="skuld-20210501" sheetId="1" r:id="rId1"/>
@@ -1639,10 +1639,10 @@
   <dimension ref="A1:M98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1712,14 +1712,14 @@
       </c>
       <c r="E2" s="1">
         <f ca="1">dates!$B$3+D2-1</f>
-        <v>44342</v>
+        <v>44373</v>
       </c>
       <c r="F2" s="16">
         <v>21</v>
       </c>
       <c r="G2" s="1">
         <f ca="1">IF(F2&gt;=D2,dates!$B$3+F2-1,dates!$B$6+F2-1)</f>
-        <v>44368</v>
+        <v>44398</v>
       </c>
       <c r="H2" s="1" t="b">
         <f ca="1">OR(E2&lt;dates!$B$3,E2&gt;dates!$B$4)</f>
@@ -1729,8 +1729,8 @@
         <v>8</v>
       </c>
       <c r="J2" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ref="J2:J33" ca="1" si="0">NOW()</f>
+        <v>44319.453377314814</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>73</v>
@@ -1755,11 +1755,11 @@
       </c>
       <c r="E3" s="1">
         <f ca="1">dates!$B$3+D3-1</f>
-        <v>44342</v>
+        <v>44373</v>
       </c>
       <c r="G3" s="1">
         <f ca="1">E3+7</f>
-        <v>44349</v>
+        <v>44380</v>
       </c>
       <c r="H3" s="1" t="b">
         <f ca="1">OR(E3&lt;dates!$B$3,E3&gt;dates!$B$4)</f>
@@ -1769,8 +1769,8 @@
         <v>8</v>
       </c>
       <c r="J3" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L3" s="1"/>
     </row>
@@ -1789,11 +1789,11 @@
       </c>
       <c r="E4" s="1">
         <f ca="1">dates!$B$3+D4-1</f>
-        <v>44342</v>
+        <v>44373</v>
       </c>
       <c r="G4" s="1">
         <f ca="1">E4+7</f>
-        <v>44349</v>
+        <v>44380</v>
       </c>
       <c r="H4" s="1" t="b">
         <f ca="1">OR(E4&lt;dates!$B$3,E4&gt;dates!$B$4)</f>
@@ -1803,8 +1803,8 @@
         <v>8</v>
       </c>
       <c r="J4" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L4" s="1"/>
     </row>
@@ -1823,14 +1823,14 @@
       </c>
       <c r="E5" s="1">
         <f ca="1">dates!$B$3+D5-1</f>
-        <v>44336</v>
+        <v>44367</v>
       </c>
       <c r="F5" s="16">
         <v>17</v>
       </c>
       <c r="G5" s="1">
         <f ca="1">IF(F5&gt;=D5,dates!$B$3+F5-1,dates!$B$6+F5-1)</f>
-        <v>44364</v>
+        <v>44394</v>
       </c>
       <c r="H5" s="1" t="b">
         <f ca="1">OR(E5&lt;dates!$B$3,E5&gt;dates!$B$4)</f>
@@ -1840,8 +1840,8 @@
         <v>8</v>
       </c>
       <c r="J5" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>69</v>
@@ -1866,11 +1866,11 @@
       </c>
       <c r="E6" s="1">
         <f ca="1">dates!$B$3+D6-1</f>
-        <v>44336</v>
+        <v>44367</v>
       </c>
       <c r="G6" s="1">
         <f ca="1">E6+7</f>
-        <v>44343</v>
+        <v>44374</v>
       </c>
       <c r="H6" s="1" t="b">
         <f ca="1">OR(E6&lt;dates!$B$3,E6&gt;dates!$B$4)</f>
@@ -1880,8 +1880,8 @@
         <v>8</v>
       </c>
       <c r="J6" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L6" s="1"/>
     </row>
@@ -1900,11 +1900,11 @@
       </c>
       <c r="E7" s="1">
         <f ca="1">dates!$B$3+D7-1</f>
-        <v>44336</v>
+        <v>44367</v>
       </c>
       <c r="G7" s="1">
         <f ca="1">E7+7</f>
-        <v>44343</v>
+        <v>44374</v>
       </c>
       <c r="H7" s="1" t="b">
         <f ca="1">OR(E7&lt;dates!$B$3,E7&gt;dates!$B$4)</f>
@@ -1914,8 +1914,8 @@
         <v>8</v>
       </c>
       <c r="J7" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L7" s="1"/>
     </row>
@@ -1934,11 +1934,11 @@
       </c>
       <c r="E8" s="1">
         <f ca="1">dates!$B$3+D8-1</f>
-        <v>44320</v>
+        <v>44351</v>
       </c>
       <c r="G8" s="1">
         <f ca="1">E8+7</f>
-        <v>44327</v>
+        <v>44358</v>
       </c>
       <c r="H8" s="1" t="b">
         <f ca="1">OR(E8&lt;dates!$B$3,E8&gt;dates!$B$4)</f>
@@ -1948,8 +1948,8 @@
         <v>8</v>
       </c>
       <c r="J8" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L8" s="1"/>
     </row>
@@ -1968,14 +1968,14 @@
       </c>
       <c r="E9" s="1">
         <f ca="1">dates!$B$3+D9-1</f>
-        <v>44319</v>
+        <v>44350</v>
       </c>
       <c r="F9" s="16">
         <v>28</v>
       </c>
       <c r="G9" s="1">
         <f ca="1">IF(F9&gt;=D9,dates!$B$3+F9-1,dates!$B$6+F9-1)</f>
-        <v>44344</v>
+        <v>44375</v>
       </c>
       <c r="H9" s="1" t="b">
         <f ca="1">OR(E9&lt;dates!$B$3,E9&gt;dates!$B$4)</f>
@@ -1985,8 +1985,8 @@
         <v>8</v>
       </c>
       <c r="J9" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>69</v>
@@ -2011,11 +2011,11 @@
       </c>
       <c r="E10" s="1">
         <f ca="1">dates!$B$3+D10-1</f>
-        <v>44320</v>
+        <v>44351</v>
       </c>
       <c r="G10" s="1">
         <f ca="1">E10+7</f>
-        <v>44327</v>
+        <v>44358</v>
       </c>
       <c r="H10" s="1" t="b">
         <f ca="1">OR(E10&lt;dates!$B$3,E10&gt;dates!$B$4)</f>
@@ -2025,8 +2025,8 @@
         <v>8</v>
       </c>
       <c r="J10" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L10" s="1"/>
     </row>
@@ -2062,8 +2062,8 @@
         <v>8</v>
       </c>
       <c r="J11" s="19">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K11" s="19" t="s">
         <v>71</v>
@@ -2091,14 +2091,14 @@
       </c>
       <c r="E12" s="1">
         <f ca="1">dates!$B$3+D12-1</f>
-        <v>44337</v>
+        <v>44368</v>
       </c>
       <c r="F12" s="16">
         <v>25</v>
       </c>
       <c r="G12" s="1">
         <f ca="1">IF(F12&gt;=D12,dates!$B$3+F12-1,dates!$B$6+F12-1)</f>
-        <v>44341</v>
+        <v>44372</v>
       </c>
       <c r="H12" s="1" t="b">
         <f ca="1">OR(E12&lt;dates!$B$3,E12&gt;dates!$B$4)</f>
@@ -2108,8 +2108,8 @@
         <v>8</v>
       </c>
       <c r="J12" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>71</v>
@@ -2134,14 +2134,14 @@
       </c>
       <c r="E13" s="1">
         <f ca="1">dates!$B$3+D13-1</f>
-        <v>44336</v>
+        <v>44367</v>
       </c>
       <c r="F13" s="16">
         <v>16</v>
       </c>
       <c r="G13" s="1">
         <f ca="1">IF(F13&gt;=D13,dates!$B$3+F13-1,dates!$B$6+F13-1)</f>
-        <v>44363</v>
+        <v>44393</v>
       </c>
       <c r="H13" s="1" t="b">
         <f ca="1">OR(E13&lt;dates!$B$3,E13&gt;dates!$B$4)</f>
@@ -2151,8 +2151,8 @@
         <v>8</v>
       </c>
       <c r="J13" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>69</v>
@@ -2177,11 +2177,11 @@
       </c>
       <c r="E14" s="1">
         <f ca="1">dates!$B$3+D14-1</f>
-        <v>44336</v>
+        <v>44367</v>
       </c>
       <c r="G14" s="1">
         <f ca="1">E14+7</f>
-        <v>44343</v>
+        <v>44374</v>
       </c>
       <c r="H14" s="1" t="b">
         <f ca="1">OR(E14&lt;dates!$B$3,E14&gt;dates!$B$4)</f>
@@ -2191,8 +2191,8 @@
         <v>8</v>
       </c>
       <c r="J14" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L14" s="1"/>
     </row>
@@ -2211,11 +2211,11 @@
       </c>
       <c r="E15" s="1">
         <f ca="1">dates!$B$3+D15-1</f>
-        <v>44336</v>
+        <v>44367</v>
       </c>
       <c r="G15" s="1">
         <f ca="1">E15+7</f>
-        <v>44343</v>
+        <v>44374</v>
       </c>
       <c r="H15" s="1" t="b">
         <f ca="1">OR(E15&lt;dates!$B$3,E15&gt;dates!$B$4)</f>
@@ -2225,8 +2225,8 @@
         <v>8</v>
       </c>
       <c r="J15" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L15" s="1"/>
     </row>
@@ -2245,14 +2245,14 @@
       </c>
       <c r="E16" s="1">
         <f ca="1">dates!$B$3+D16-1</f>
-        <v>44339</v>
+        <v>44370</v>
       </c>
       <c r="F16" s="16">
         <v>20</v>
       </c>
       <c r="G16" s="1">
         <f ca="1">IF(F16&gt;=D16,dates!$B$3+F16-1,dates!$B$6+F16-1)</f>
-        <v>44367</v>
+        <v>44397</v>
       </c>
       <c r="H16" s="1" t="b">
         <f ca="1">OR(E16&lt;dates!$B$3,E16&gt;dates!$B$4)</f>
@@ -2262,8 +2262,8 @@
         <v>8</v>
       </c>
       <c r="J16" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>69</v>
@@ -2288,11 +2288,11 @@
       </c>
       <c r="E17" s="1">
         <f ca="1">dates!$B$3+D17-1</f>
-        <v>44340</v>
+        <v>44371</v>
       </c>
       <c r="G17" s="1">
         <f ca="1">E17+7</f>
-        <v>44347</v>
+        <v>44378</v>
       </c>
       <c r="H17" s="1" t="b">
         <f ca="1">OR(E17&lt;dates!$B$3,E17&gt;dates!$B$4)</f>
@@ -2302,8 +2302,8 @@
         <v>8</v>
       </c>
       <c r="J17" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L17" s="1"/>
     </row>
@@ -2322,11 +2322,11 @@
       </c>
       <c r="E18" s="1">
         <f ca="1">dates!$B$3+D18-1</f>
-        <v>44340</v>
+        <v>44371</v>
       </c>
       <c r="G18" s="1">
         <f ca="1">E18+7</f>
-        <v>44347</v>
+        <v>44378</v>
       </c>
       <c r="H18" s="1" t="b">
         <f ca="1">OR(E18&lt;dates!$B$3,E18&gt;dates!$B$4)</f>
@@ -2336,8 +2336,8 @@
         <v>8</v>
       </c>
       <c r="J18" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L18" s="1"/>
     </row>
@@ -2353,19 +2353,19 @@
       </c>
       <c r="D19" s="16">
         <f ca="1">F19-7</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E19" s="1">
         <f ca="1">dates!$B$3+D19-1</f>
-        <v>44340</v>
+        <v>44370</v>
       </c>
       <c r="F19" s="16">
         <f ca="1">dates!B4-dates!B3+1</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G19" s="19">
         <f ca="1">IF(F19&gt;=D19,dates!$B$3+F19-1,dates!$B$6+F19-1)</f>
-        <v>44347</v>
+        <v>44377</v>
       </c>
       <c r="H19" s="1" t="b">
         <f ca="1">OR(E19&lt;dates!$B$3,E19&gt;dates!$B$4)</f>
@@ -2375,8 +2375,8 @@
         <v>8</v>
       </c>
       <c r="J19" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L19" t="s">
         <v>121</v>
@@ -2394,18 +2394,18 @@
       </c>
       <c r="D20">
         <f ca="1">DAY(dates!$B$4)</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E20" s="1">
         <f ca="1">dates!$B$4</f>
-        <v>44347</v>
+        <v>44377</v>
       </c>
       <c r="F20" s="16">
         <v>7</v>
       </c>
       <c r="G20" s="1">
         <f ca="1">IF(F20&gt;=D20,dates!$B$3+F20-1,dates!$B$6+F20-1)</f>
-        <v>44354</v>
+        <v>44384</v>
       </c>
       <c r="H20" s="1" t="b">
         <f ca="1">OR(E20&lt;dates!$B$3,E20&gt;dates!$B$4)</f>
@@ -2415,8 +2415,8 @@
         <v>8</v>
       </c>
       <c r="J20" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>74</v>
@@ -2442,12 +2442,12 @@
       </c>
       <c r="E21" s="1">
         <f ca="1">dates!$B$3+D21-1</f>
-        <v>44317</v>
+        <v>44348</v>
       </c>
       <c r="F21" s="16"/>
       <c r="G21" s="1">
         <f ca="1">E21+7</f>
-        <v>44324</v>
+        <v>44355</v>
       </c>
       <c r="H21" s="1" t="b">
         <f ca="1">OR(E21&lt;dates!$B$3,E21&gt;dates!$B$4)</f>
@@ -2457,8 +2457,8 @@
         <v>8</v>
       </c>
       <c r="J21" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -2479,11 +2479,11 @@
       </c>
       <c r="E22" s="1">
         <f ca="1">dates!$B$3+D22-1</f>
-        <v>44317</v>
+        <v>44348</v>
       </c>
       <c r="G22" s="1">
         <f ca="1">E22+7</f>
-        <v>44324</v>
+        <v>44355</v>
       </c>
       <c r="H22" s="1" t="b">
         <f ca="1">OR(E22&lt;dates!$B$3,E22&gt;dates!$B$4)</f>
@@ -2493,8 +2493,8 @@
         <v>8</v>
       </c>
       <c r="J22" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L22" s="1"/>
     </row>
@@ -2510,18 +2510,18 @@
       </c>
       <c r="D23">
         <f ca="1">DAY(dates!$B$4)</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E23" s="1">
         <f ca="1">dates!$B$4</f>
-        <v>44347</v>
+        <v>44377</v>
       </c>
       <c r="F23" s="16">
         <v>7</v>
       </c>
       <c r="G23" s="1">
         <f ca="1">IF(F23&gt;=D23,dates!$B$3+F23-1,dates!$B$6+F23-1)</f>
-        <v>44354</v>
+        <v>44384</v>
       </c>
       <c r="H23" s="1" t="b">
         <f ca="1">OR(E23&lt;dates!$B$3,E23&gt;dates!$B$4)</f>
@@ -2531,8 +2531,8 @@
         <v>8</v>
       </c>
       <c r="J23" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>74</v>
@@ -2558,12 +2558,12 @@
       </c>
       <c r="E24" s="1">
         <f ca="1">dates!$B$3+D24-1</f>
-        <v>44317</v>
+        <v>44348</v>
       </c>
       <c r="F24" s="16"/>
       <c r="G24" s="1">
         <f ca="1">E24+7</f>
-        <v>44324</v>
+        <v>44355</v>
       </c>
       <c r="H24" s="1" t="b">
         <f ca="1">OR(E24&lt;dates!$B$3,E24&gt;dates!$B$4)</f>
@@ -2573,8 +2573,8 @@
         <v>8</v>
       </c>
       <c r="J24" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -2595,12 +2595,12 @@
       </c>
       <c r="E25" s="1">
         <f ca="1">dates!$B$3+D25-1</f>
-        <v>44317</v>
+        <v>44348</v>
       </c>
       <c r="F25" s="16"/>
       <c r="G25" s="1">
         <f ca="1">E25+7</f>
-        <v>44324</v>
+        <v>44355</v>
       </c>
       <c r="H25" s="1" t="b">
         <f ca="1">OR(E25&lt;dates!$B$3,E25&gt;dates!$B$4)</f>
@@ -2610,8 +2610,8 @@
         <v>8</v>
       </c>
       <c r="J25" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -2632,14 +2632,14 @@
       </c>
       <c r="E26" s="1">
         <f ca="1">dates!$B$3+D26-1</f>
-        <v>44344</v>
+        <v>44375</v>
       </c>
       <c r="F26" s="16">
         <v>23</v>
       </c>
       <c r="G26" s="1">
         <f ca="1">IF(F26&gt;=D26,dates!$B$3+F26-1,dates!$B$6+F26-1)</f>
-        <v>44370</v>
+        <v>44400</v>
       </c>
       <c r="H26" s="1" t="b">
         <f ca="1">OR(E26&lt;dates!$B$3,E26&gt;dates!$B$4)</f>
@@ -2649,8 +2649,8 @@
         <v>8</v>
       </c>
       <c r="J26" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>69</v>
@@ -2672,18 +2672,18 @@
         <v>9</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E27" s="1">
         <f ca="1">dates!$B$3+D27-1</f>
-        <v>44317</v>
+        <v>44350</v>
       </c>
       <c r="F27" s="16">
         <v>7</v>
       </c>
       <c r="G27" s="1">
         <f ca="1">E27+7-1</f>
-        <v>44323</v>
+        <v>44356</v>
       </c>
       <c r="H27" s="1" t="b">
         <f ca="1">OR(E27&lt;dates!$B$3,E27&gt;dates!$B$4)</f>
@@ -2693,8 +2693,8 @@
         <v>8</v>
       </c>
       <c r="J27" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L27" s="1"/>
     </row>
@@ -2713,11 +2713,11 @@
       </c>
       <c r="E28" s="1">
         <f ca="1">dates!$B$3+D28-1</f>
-        <v>44344</v>
+        <v>44375</v>
       </c>
       <c r="G28" s="1">
         <f ca="1">E28+7</f>
-        <v>44351</v>
+        <v>44382</v>
       </c>
       <c r="H28" s="1" t="b">
         <f ca="1">OR(E28&lt;dates!$B$3,E28&gt;dates!$B$4)</f>
@@ -2727,8 +2727,8 @@
         <v>8</v>
       </c>
       <c r="J28" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L28" s="1"/>
     </row>
@@ -2764,8 +2764,8 @@
         <v>8</v>
       </c>
       <c r="J29" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>71</v>
@@ -2793,14 +2793,14 @@
       </c>
       <c r="E30" s="1">
         <f ca="1">dates!$B$3+D30-1</f>
-        <v>44333</v>
+        <v>44364</v>
       </c>
       <c r="F30" s="16">
         <v>13</v>
       </c>
       <c r="G30" s="1">
         <f ca="1">IF(F30&gt;=D30,dates!$B$3+F30-1,dates!$B$6+F30-1)</f>
-        <v>44360</v>
+        <v>44390</v>
       </c>
       <c r="H30" s="1" t="b">
         <f ca="1">OR(E30&lt;dates!$B$3,E30&gt;dates!$B$4)</f>
@@ -2810,8 +2810,8 @@
         <v>8</v>
       </c>
       <c r="J30" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>69</v>
@@ -2836,11 +2836,11 @@
       </c>
       <c r="E31" s="1">
         <f ca="1">dates!$B$3+D31-1</f>
-        <v>44333</v>
+        <v>44364</v>
       </c>
       <c r="G31" s="1">
         <f ca="1">E31+7</f>
-        <v>44340</v>
+        <v>44371</v>
       </c>
       <c r="H31" s="1" t="b">
         <f ca="1">OR(E31&lt;dates!$B$3,E31&gt;dates!$B$4)</f>
@@ -2850,8 +2850,8 @@
         <v>8</v>
       </c>
       <c r="J31" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L31" s="1"/>
     </row>
@@ -2870,11 +2870,11 @@
       </c>
       <c r="E32" s="1">
         <f ca="1">dates!$B$3+D32-1</f>
-        <v>44333</v>
+        <v>44364</v>
       </c>
       <c r="G32" s="1">
         <f ca="1">E32+7</f>
-        <v>44340</v>
+        <v>44371</v>
       </c>
       <c r="H32" s="1" t="b">
         <f ca="1">OR(E32&lt;dates!$B$3,E32&gt;dates!$B$4)</f>
@@ -2884,8 +2884,8 @@
         <v>8</v>
       </c>
       <c r="J32" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L32" s="1"/>
     </row>
@@ -2921,8 +2921,8 @@
         <v>8</v>
       </c>
       <c r="J33" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L33" s="1" t="str">
         <f>"S/S: "&amp;K33</f>
@@ -2947,14 +2947,14 @@
       </c>
       <c r="E34" s="1">
         <f ca="1">dates!$B$3+D34-1</f>
-        <v>44330</v>
+        <v>44361</v>
       </c>
       <c r="F34" s="16">
         <v>7</v>
       </c>
       <c r="G34" s="1">
         <f ca="1">IF(F34&gt;=D34,dates!$B$3+F34-1,dates!$B$6+F34-1)</f>
-        <v>44354</v>
+        <v>44384</v>
       </c>
       <c r="H34" s="1" t="b">
         <f ca="1">OR(E34&lt;dates!$B$3,E34&gt;dates!$B$4)</f>
@@ -2964,8 +2964,8 @@
         <v>8</v>
       </c>
       <c r="J34" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ref="J34:J65" ca="1" si="1">NOW()</f>
+        <v>44319.453377314814</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>69</v>
@@ -2990,11 +2990,11 @@
       </c>
       <c r="E35" s="1">
         <f ca="1">dates!$B$3+D35-1</f>
-        <v>44330</v>
+        <v>44361</v>
       </c>
       <c r="G35" s="1">
         <f ca="1">E35+7</f>
-        <v>44337</v>
+        <v>44368</v>
       </c>
       <c r="H35" s="1" t="b">
         <f ca="1">OR(E35&lt;dates!$B$3,E35&gt;dates!$B$4)</f>
@@ -3004,8 +3004,8 @@
         <v>8</v>
       </c>
       <c r="J35" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L35" s="1"/>
     </row>
@@ -3024,11 +3024,11 @@
       </c>
       <c r="E36" s="1">
         <f ca="1">dates!$B$3+D36-1</f>
-        <v>44330</v>
+        <v>44361</v>
       </c>
       <c r="G36" s="1">
         <f ca="1">E36+7</f>
-        <v>44337</v>
+        <v>44368</v>
       </c>
       <c r="H36" s="1" t="b">
         <f ca="1">OR(E36&lt;dates!$B$3,E36&gt;dates!$B$4)</f>
@@ -3038,8 +3038,8 @@
         <v>8</v>
       </c>
       <c r="J36" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L36" s="1"/>
     </row>
@@ -3075,8 +3075,8 @@
         <v>8</v>
       </c>
       <c r="J37" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>76</v>
@@ -3104,14 +3104,14 @@
       </c>
       <c r="E38" s="1">
         <f ca="1">dates!$B$3+D38-1</f>
-        <v>44333</v>
+        <v>44364</v>
       </c>
       <c r="F38" s="16">
         <v>10</v>
       </c>
       <c r="G38" s="1">
         <f ca="1">IF(F38&gt;=D38,dates!$B$3+F38-1,dates!$B$6+F38-1)</f>
-        <v>44357</v>
+        <v>44387</v>
       </c>
       <c r="H38" s="1" t="b">
         <f ca="1">OR(E38&lt;dates!$B$3,E38&gt;dates!$B$4)</f>
@@ -3121,8 +3121,8 @@
         <v>8</v>
       </c>
       <c r="J38" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>69</v>
@@ -3147,14 +3147,14 @@
       </c>
       <c r="E39" s="1">
         <f ca="1">dates!$B$3+D39-1</f>
-        <v>44344</v>
+        <v>44375</v>
       </c>
       <c r="F39" s="16">
         <v>28</v>
       </c>
       <c r="G39" s="1">
         <f ca="1">IF(F39&gt;=D39,dates!$B$3+F39-1,dates!$B$6+F39-1)</f>
-        <v>44344</v>
+        <v>44375</v>
       </c>
       <c r="H39" s="1" t="b">
         <f ca="1">OR(E39&lt;dates!$B$3,E39&gt;dates!$B$4)</f>
@@ -3164,8 +3164,8 @@
         <v>8</v>
       </c>
       <c r="J39" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>69</v>
@@ -3190,14 +3190,14 @@
       </c>
       <c r="E40" s="1">
         <f ca="1">dates!$B$3+D40-1</f>
-        <v>44344</v>
+        <v>44375</v>
       </c>
       <c r="F40" s="16">
         <v>28</v>
       </c>
       <c r="G40" s="1">
         <f ca="1">IF(F40&gt;=D40,dates!$B$3+F40-1,dates!$B$6+F40-1)</f>
-        <v>44344</v>
+        <v>44375</v>
       </c>
       <c r="H40" s="1" t="b">
         <f ca="1">OR(E40&lt;dates!$B$3,E40&gt;dates!$B$4)</f>
@@ -3207,8 +3207,8 @@
         <v>8</v>
       </c>
       <c r="J40" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>69</v>
@@ -3250,8 +3250,8 @@
         <v>8</v>
       </c>
       <c r="J41" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="M41">
         <v>1</v>
@@ -3289,8 +3289,8 @@
         <v>8</v>
       </c>
       <c r="J42" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>69</v>
@@ -3318,14 +3318,14 @@
       </c>
       <c r="E43" s="1">
         <f ca="1">dates!$B$3+D43-1</f>
-        <v>44317</v>
+        <v>44348</v>
       </c>
       <c r="F43" s="16">
         <v>1</v>
       </c>
       <c r="G43" s="1">
         <f ca="1">IF(F43&gt;=D43,dates!$B$3+F43-1,dates!$B$6+F43-1)</f>
-        <v>44317</v>
+        <v>44348</v>
       </c>
       <c r="H43" s="1" t="b">
         <f ca="1">OR(E43&lt;dates!$B$3,E43&gt;dates!$B$4)</f>
@@ -3335,8 +3335,8 @@
         <v>8</v>
       </c>
       <c r="J43" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>71</v>
@@ -3361,14 +3361,14 @@
       </c>
       <c r="E44" s="1">
         <f ca="1">dates!$B$3+D44-1</f>
-        <v>44324</v>
+        <v>44355</v>
       </c>
       <c r="F44" s="16">
         <v>19</v>
       </c>
       <c r="G44" s="1">
         <f ca="1">IF(F44&gt;=D44,dates!$B$3+F44-1,dates!$B$6+F44-1)</f>
-        <v>44335</v>
+        <v>44366</v>
       </c>
       <c r="H44" s="1" t="b">
         <f ca="1">OR(E44&lt;dates!$B$3,E44&gt;dates!$B$4)</f>
@@ -3378,8 +3378,8 @@
         <v>8</v>
       </c>
       <c r="J44" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>71</v>
@@ -3404,14 +3404,14 @@
       </c>
       <c r="E45" s="1">
         <f ca="1">dates!$B$3+D45-1</f>
-        <v>44324</v>
+        <v>44355</v>
       </c>
       <c r="F45" s="16">
         <v>8</v>
       </c>
       <c r="G45" s="1">
         <f ca="1">IF(F45&gt;=D45,dates!$B$3+F45-1,dates!$B$6+F45-1)</f>
-        <v>44324</v>
+        <v>44355</v>
       </c>
       <c r="H45" s="1" t="b">
         <f ca="1">OR(E45&lt;dates!$B$3,E45&gt;dates!$B$4)</f>
@@ -3421,8 +3421,8 @@
         <v>8</v>
       </c>
       <c r="J45" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>71</v>
@@ -3465,8 +3465,8 @@
         <v>8</v>
       </c>
       <c r="J46" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K46" s="1" t="s">
         <v>71</v>
@@ -3511,8 +3511,8 @@
         <v>8</v>
       </c>
       <c r="J47" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>71</v>
@@ -3553,8 +3553,8 @@
         <v>8</v>
       </c>
       <c r="J48" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K48" s="1" t="s">
         <v>71</v>
@@ -3599,8 +3599,8 @@
         <v>8</v>
       </c>
       <c r="J49" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K49" s="1" t="s">
         <v>69</v>
@@ -3645,8 +3645,8 @@
         <v>8</v>
       </c>
       <c r="J50" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>69</v>
@@ -3674,14 +3674,14 @@
       </c>
       <c r="E51" s="1">
         <f ca="1">dates!$B$3+D51-1</f>
-        <v>44333</v>
+        <v>44364</v>
       </c>
       <c r="F51" s="16">
         <v>13</v>
       </c>
       <c r="G51" s="1">
         <f ca="1">IF(F51&gt;=D51,dates!$B$3+F51-1,dates!$B$6+F51-1)</f>
-        <v>44360</v>
+        <v>44390</v>
       </c>
       <c r="H51" s="1" t="b">
         <f ca="1">OR(E51&lt;dates!$B$3,E51&gt;dates!$B$4)</f>
@@ -3691,8 +3691,8 @@
         <v>8</v>
       </c>
       <c r="J51" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K51" s="1" t="s">
         <v>69</v>
@@ -3717,11 +3717,11 @@
       </c>
       <c r="E52" s="1">
         <f ca="1">dates!$B$3+D52-1</f>
-        <v>44338</v>
+        <v>44369</v>
       </c>
       <c r="G52" s="1">
         <f ca="1">E52+7</f>
-        <v>44345</v>
+        <v>44376</v>
       </c>
       <c r="H52" s="1" t="b">
         <f ca="1">OR(E52&lt;dates!$B$3,E52&gt;dates!$B$4)</f>
@@ -3731,8 +3731,8 @@
         <v>8</v>
       </c>
       <c r="J52" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L52" s="1"/>
     </row>
@@ -3751,11 +3751,11 @@
       </c>
       <c r="E53" s="1">
         <f ca="1">dates!$B$3+D53-1</f>
-        <v>44338</v>
+        <v>44369</v>
       </c>
       <c r="G53" s="1">
         <f ca="1">E53+7</f>
-        <v>44345</v>
+        <v>44376</v>
       </c>
       <c r="H53" s="1" t="b">
         <f ca="1">OR(E53&lt;dates!$B$3,E53&gt;dates!$B$4)</f>
@@ -3765,8 +3765,8 @@
         <v>8</v>
       </c>
       <c r="J53" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L53" s="1"/>
     </row>
@@ -3785,14 +3785,14 @@
       </c>
       <c r="E54" s="1">
         <f ca="1">dates!$B$3+D54-1</f>
-        <v>44326</v>
+        <v>44357</v>
       </c>
       <c r="F54" s="16">
         <v>10</v>
       </c>
       <c r="G54" s="1">
         <f ca="1">IF(F54&gt;=D54,dates!$B$3+F54-1,dates!$B$6+F54-1)</f>
-        <v>44326</v>
+        <v>44357</v>
       </c>
       <c r="H54" s="1" t="b">
         <f ca="1">OR(E54&lt;dates!$B$3,E54&gt;dates!$B$4)</f>
@@ -3802,8 +3802,8 @@
         <v>8</v>
       </c>
       <c r="J54" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>76</v>
@@ -3828,14 +3828,14 @@
       </c>
       <c r="E55" s="1">
         <f ca="1">dates!$B$3+D55-1</f>
-        <v>44317</v>
+        <v>44348</v>
       </c>
       <c r="F55" s="16">
         <v>7</v>
       </c>
       <c r="G55" s="1">
         <f ca="1">IF(F55&gt;=D55,dates!$B$3+F55-1,dates!$B$6+F55-1)</f>
-        <v>44323</v>
+        <v>44354</v>
       </c>
       <c r="H55" s="1" t="b">
         <f ca="1">OR(E55&lt;dates!$B$3,E55&gt;dates!$B$4)</f>
@@ -3845,8 +3845,8 @@
         <v>8</v>
       </c>
       <c r="J55" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
@@ -3864,14 +3864,14 @@
       </c>
       <c r="E56" s="1">
         <f ca="1">dates!$B$3+D56-1</f>
-        <v>44317</v>
+        <v>44348</v>
       </c>
       <c r="F56" s="16">
         <v>7</v>
       </c>
       <c r="G56" s="1">
         <f ca="1">IF(F56&gt;=D56,dates!$B$3+F56-1,dates!$B$6+F56-1)</f>
-        <v>44323</v>
+        <v>44354</v>
       </c>
       <c r="H56" s="1" t="b">
         <f ca="1">OR(E56&lt;dates!$B$3,E56&gt;dates!$B$4)</f>
@@ -3881,8 +3881,8 @@
         <v>8</v>
       </c>
       <c r="J56" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
@@ -3900,14 +3900,14 @@
       </c>
       <c r="E57" s="1">
         <f ca="1">dates!$B$3+D57-1</f>
-        <v>44317</v>
+        <v>44348</v>
       </c>
       <c r="F57" s="16">
         <v>7</v>
       </c>
       <c r="G57" s="1">
         <f ca="1">IF(F57&gt;=D57,dates!$B$3+F57-1,dates!$B$6+F57-1)</f>
-        <v>44323</v>
+        <v>44354</v>
       </c>
       <c r="H57" s="1" t="b">
         <f ca="1">OR(E57&lt;dates!$B$3,E57&gt;dates!$B$4)</f>
@@ -3917,8 +3917,8 @@
         <v>8</v>
       </c>
       <c r="J57" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -3933,18 +3933,18 @@
       </c>
       <c r="D58" s="18">
         <f ca="1">DAY(dates!$B$4)</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E58" s="19">
         <f ca="1">dates!$B$4</f>
-        <v>44347</v>
+        <v>44377</v>
       </c>
       <c r="F58" s="20">
         <v>7</v>
       </c>
       <c r="G58" s="19">
         <f ca="1">E58+7</f>
-        <v>44354</v>
+        <v>44384</v>
       </c>
       <c r="H58" s="1" t="b">
         <f ca="1">OR(E58&lt;dates!$B$3,E58&gt;dates!$B$4)</f>
@@ -3954,8 +3954,8 @@
         <v>8</v>
       </c>
       <c r="J58" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K58" s="19" t="s">
         <v>69</v>
@@ -3981,12 +3981,12 @@
       </c>
       <c r="E59" s="1">
         <f ca="1">dates!$B$3+D59-1</f>
-        <v>44317</v>
+        <v>44348</v>
       </c>
       <c r="F59" s="20"/>
       <c r="G59" s="1">
         <f ca="1">E59+7-1</f>
-        <v>44323</v>
+        <v>44354</v>
       </c>
       <c r="H59" s="1" t="b">
         <f ca="1">OR(E59&lt;dates!$B$3,E59&gt;dates!$B$4)</f>
@@ -3996,8 +3996,8 @@
         <v>8</v>
       </c>
       <c r="J59" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K59" s="19"/>
       <c r="L59" s="19"/>
@@ -4018,12 +4018,12 @@
       </c>
       <c r="E60" s="1">
         <f ca="1">dates!$B$3+D60-1</f>
-        <v>44317</v>
+        <v>44348</v>
       </c>
       <c r="F60" s="20"/>
       <c r="G60" s="1">
         <f ca="1">E60+7</f>
-        <v>44324</v>
+        <v>44355</v>
       </c>
       <c r="H60" s="1" t="b">
         <f ca="1">OR(E60&lt;dates!$B$3,E60&gt;dates!$B$4)</f>
@@ -4033,8 +4033,8 @@
         <v>8</v>
       </c>
       <c r="J60" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K60" s="19"/>
       <c r="L60" s="19"/>
@@ -4055,14 +4055,14 @@
       </c>
       <c r="E61" s="1">
         <f ca="1">dates!$B$3+D61-1</f>
-        <v>44317</v>
+        <v>44348</v>
       </c>
       <c r="F61" s="16">
         <v>7</v>
       </c>
       <c r="G61" s="1">
         <f ca="1">IF(F61&gt;=D61,dates!$B$3+F61-1,dates!$B$6+F61-1)</f>
-        <v>44323</v>
+        <v>44354</v>
       </c>
       <c r="H61" s="1" t="b">
         <f ca="1">OR(E61&lt;dates!$B$3,E61&gt;dates!$B$4)</f>
@@ -4072,8 +4072,8 @@
         <v>8</v>
       </c>
       <c r="J61" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
@@ -4091,14 +4091,14 @@
       </c>
       <c r="E62" s="1">
         <f ca="1">dates!$B$3+D62-1</f>
-        <v>44317</v>
+        <v>44348</v>
       </c>
       <c r="F62" s="16">
         <v>7</v>
       </c>
       <c r="G62" s="1">
         <f ca="1">IF(F62&gt;=D62,dates!$B$3+F62-1,dates!$B$6+F62-1)</f>
-        <v>44323</v>
+        <v>44354</v>
       </c>
       <c r="H62" s="1" t="b">
         <f ca="1">OR(E62&lt;dates!$B$3,E62&gt;dates!$B$4)</f>
@@ -4108,8 +4108,8 @@
         <v>8</v>
       </c>
       <c r="J62" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
@@ -4127,14 +4127,14 @@
       </c>
       <c r="E63" s="1">
         <f ca="1">dates!$B$3+D63-1</f>
-        <v>44317</v>
+        <v>44348</v>
       </c>
       <c r="F63" s="16">
         <v>7</v>
       </c>
       <c r="G63" s="1">
         <f ca="1">IF(F63&gt;=D63,dates!$B$3+F63-1,dates!$B$6+F63-1)</f>
-        <v>44323</v>
+        <v>44354</v>
       </c>
       <c r="H63" s="1" t="b">
         <f ca="1">OR(E63&lt;dates!$B$3,E63&gt;dates!$B$4)</f>
@@ -4144,8 +4144,8 @@
         <v>8</v>
       </c>
       <c r="J63" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
@@ -4163,14 +4163,14 @@
       </c>
       <c r="E64" s="1">
         <f ca="1">dates!$B$3+D64-1</f>
-        <v>44323</v>
+        <v>44354</v>
       </c>
       <c r="F64" s="16">
         <v>14</v>
       </c>
       <c r="G64" s="1">
         <f ca="1">IF(F64&gt;=D64,dates!$B$3+F64-1,dates!$B$6+F64-1)</f>
-        <v>44330</v>
+        <v>44361</v>
       </c>
       <c r="H64" s="1" t="b">
         <f ca="1">OR(E64&lt;dates!$B$3,E64&gt;dates!$B$4)</f>
@@ -4180,8 +4180,8 @@
         <v>8</v>
       </c>
       <c r="J64" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
@@ -4199,14 +4199,14 @@
       </c>
       <c r="E65" s="1">
         <f ca="1">dates!$B$3+D65-1</f>
-        <v>44323</v>
+        <v>44354</v>
       </c>
       <c r="F65" s="16">
         <v>14</v>
       </c>
       <c r="G65" s="1">
         <f ca="1">IF(F65&gt;=D65,dates!$B$3+F65-1,dates!$B$6+F65-1)</f>
-        <v>44330</v>
+        <v>44361</v>
       </c>
       <c r="H65" s="1" t="b">
         <f ca="1">OR(E65&lt;dates!$B$3,E65&gt;dates!$B$4)</f>
@@ -4216,8 +4216,8 @@
         <v>8</v>
       </c>
       <c r="J65" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44319.453377314814</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
@@ -4235,14 +4235,14 @@
       </c>
       <c r="E66" s="1">
         <f ca="1">dates!$B$3+D66-1</f>
-        <v>44323</v>
+        <v>44354</v>
       </c>
       <c r="F66" s="16">
         <v>14</v>
       </c>
       <c r="G66" s="1">
         <f ca="1">IF(F66&gt;=D66,dates!$B$3+F66-1,dates!$B$6+F66-1)</f>
-        <v>44330</v>
+        <v>44361</v>
       </c>
       <c r="H66" s="1" t="b">
         <f ca="1">OR(E66&lt;dates!$B$3,E66&gt;dates!$B$4)</f>
@@ -4252,8 +4252,8 @@
         <v>8</v>
       </c>
       <c r="J66" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ref="J66:J98" ca="1" si="2">NOW()</f>
+        <v>44319.453377314814</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
@@ -4271,14 +4271,14 @@
       </c>
       <c r="E67" s="1">
         <f ca="1">dates!$B$3+D67-1</f>
-        <v>44323</v>
+        <v>44354</v>
       </c>
       <c r="F67" s="16">
         <v>14</v>
       </c>
       <c r="G67" s="1">
         <f ca="1">IF(F67&gt;=D67,dates!$B$3+F67-1,dates!$B$6+F67-1)</f>
-        <v>44330</v>
+        <v>44361</v>
       </c>
       <c r="H67" s="1" t="b">
         <f ca="1">OR(E67&lt;dates!$B$3,E67&gt;dates!$B$4)</f>
@@ -4288,8 +4288,8 @@
         <v>8</v>
       </c>
       <c r="J67" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
     </row>
     <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
@@ -4324,8 +4324,8 @@
         <v>8</v>
       </c>
       <c r="J68" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K68" s="19" t="s">
         <v>69</v>
@@ -4353,14 +4353,14 @@
       </c>
       <c r="E69" s="1">
         <f ca="1">dates!$B$3+D69-1</f>
-        <v>44333</v>
+        <v>44364</v>
       </c>
       <c r="F69" s="16">
         <v>17</v>
       </c>
       <c r="G69" s="1">
         <f ca="1">IF(F69&gt;=D69,dates!$B$3+F69-1,dates!$B$6+F69-1)</f>
-        <v>44333</v>
+        <v>44364</v>
       </c>
       <c r="H69" s="1" t="b">
         <f ca="1">OR(E69&lt;dates!$B$3,E69&gt;dates!$B$4)</f>
@@ -4370,8 +4370,8 @@
         <v>8</v>
       </c>
       <c r="J69" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K69" s="1" t="s">
         <v>77</v>
@@ -4396,14 +4396,14 @@
       </c>
       <c r="E70" s="1">
         <f ca="1">dates!$B$3+D70-1</f>
-        <v>44336</v>
+        <v>44367</v>
       </c>
       <c r="F70" s="16">
         <v>17</v>
       </c>
       <c r="G70" s="1">
         <f ca="1">IF(F70&gt;=D70,dates!$B$3+F70-1,dates!$B$6+F70-1)</f>
-        <v>44364</v>
+        <v>44394</v>
       </c>
       <c r="H70" s="1" t="b">
         <f ca="1">OR(E70&lt;dates!$B$3,E70&gt;dates!$B$4)</f>
@@ -4413,8 +4413,8 @@
         <v>8</v>
       </c>
       <c r="J70" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K70" s="1" t="s">
         <v>69</v>
@@ -4439,11 +4439,11 @@
       </c>
       <c r="E71" s="1">
         <f ca="1">dates!$B$3+D71-1</f>
-        <v>44337</v>
+        <v>44368</v>
       </c>
       <c r="G71" s="1">
         <f ca="1">E71+7</f>
-        <v>44344</v>
+        <v>44375</v>
       </c>
       <c r="H71" s="1" t="b">
         <f ca="1">OR(E71&lt;dates!$B$3,E71&gt;dates!$B$4)</f>
@@ -4453,8 +4453,8 @@
         <v>8</v>
       </c>
       <c r="J71" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L71" s="1"/>
     </row>
@@ -4473,11 +4473,11 @@
       </c>
       <c r="E72" s="1">
         <f ca="1">dates!$B$3+D72-1</f>
-        <v>44337</v>
+        <v>44368</v>
       </c>
       <c r="G72" s="1">
         <f ca="1">E72+7</f>
-        <v>44344</v>
+        <v>44375</v>
       </c>
       <c r="H72" s="1" t="b">
         <f ca="1">OR(E72&lt;dates!$B$3,E72&gt;dates!$B$4)</f>
@@ -4487,8 +4487,8 @@
         <v>8</v>
       </c>
       <c r="J72" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L72" s="1"/>
     </row>
@@ -4507,14 +4507,14 @@
       </c>
       <c r="E73" s="1">
         <f ca="1">dates!$B$3+D73-1</f>
-        <v>44344</v>
+        <v>44375</v>
       </c>
       <c r="F73" s="16">
         <v>28</v>
       </c>
       <c r="G73" s="1">
         <f ca="1">E73+7</f>
-        <v>44351</v>
+        <v>44382</v>
       </c>
       <c r="H73" s="1" t="b">
         <f ca="1">OR(E73&lt;dates!$B$3,E73&gt;dates!$B$4)</f>
@@ -4524,8 +4524,8 @@
         <v>8</v>
       </c>
       <c r="J73" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K73" s="1" t="s">
         <v>71</v>
@@ -4547,11 +4547,11 @@
       </c>
       <c r="D74">
         <f ca="1">DAY(dates!$B$9)</f>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E74" s="1">
         <f ca="1">dates!$B$3+D74-1</f>
-        <v>44335</v>
+        <v>44363</v>
       </c>
       <c r="F74" s="16">
         <v>18</v>
@@ -4568,8 +4568,8 @@
         <v>8</v>
       </c>
       <c r="J74" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K74" s="1" t="s">
         <v>70</v>
@@ -4591,11 +4591,11 @@
       </c>
       <c r="D75">
         <f ca="1">DAY(dates!$B$9)</f>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E75" s="1">
         <f ca="1">dates!$B$3+D75-1</f>
-        <v>44335</v>
+        <v>44363</v>
       </c>
       <c r="F75" s="16">
         <v>18</v>
@@ -4612,8 +4612,8 @@
         <v>8</v>
       </c>
       <c r="J75" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K75" s="1" t="s">
         <v>70</v>
@@ -4639,14 +4639,14 @@
       </c>
       <c r="E76" s="1">
         <f ca="1">dates!$B$3+D76-1</f>
-        <v>44335</v>
+        <v>44366</v>
       </c>
       <c r="F76" s="16">
         <v>19</v>
       </c>
       <c r="G76" s="1">
         <f ca="1">IF(F76&gt;=D76,dates!$B$3+F76-1,dates!$B$6+F76-1)</f>
-        <v>44335</v>
+        <v>44366</v>
       </c>
       <c r="H76" s="1" t="b">
         <f ca="1">OR(E76&lt;dates!$B$3,E76&gt;dates!$B$4)</f>
@@ -4656,8 +4656,8 @@
         <v>8</v>
       </c>
       <c r="J76" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K76" s="1" t="s">
         <v>71</v>
@@ -4699,8 +4699,8 @@
         <v>8</v>
       </c>
       <c r="J77" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K77" s="1" t="s">
         <v>71</v>
@@ -4724,14 +4724,14 @@
       </c>
       <c r="E78" s="1">
         <f ca="1">dates!$B$3+D78-1</f>
-        <v>44321</v>
+        <v>44352</v>
       </c>
       <c r="F78" s="16">
         <v>5</v>
       </c>
       <c r="G78" s="1">
         <f ca="1">IF(F78&gt;=D78,dates!$B$3+F78-1,dates!$B$6+F78-1)</f>
-        <v>44321</v>
+        <v>44352</v>
       </c>
       <c r="H78" s="1" t="b">
         <f ca="1">OR(E78&lt;dates!$B$3,E78&gt;dates!$B$4)</f>
@@ -4741,8 +4741,8 @@
         <v>8</v>
       </c>
       <c r="J78" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K78" s="1" t="s">
         <v>69</v>
@@ -4767,14 +4767,14 @@
       </c>
       <c r="E79" s="1">
         <f ca="1">dates!$B$3+D79-1</f>
-        <v>44317</v>
+        <v>44348</v>
       </c>
       <c r="F79" s="16">
         <v>1</v>
       </c>
       <c r="G79" s="1">
         <f ca="1">IF(F79&gt;=D79,dates!$B$3+F79-1,dates!$B$6+F79-1)</f>
-        <v>44317</v>
+        <v>44348</v>
       </c>
       <c r="H79" s="1" t="b">
         <f ca="1">OR(E79&lt;dates!$B$3,E79&gt;dates!$B$4)</f>
@@ -4784,8 +4784,8 @@
         <v>8</v>
       </c>
       <c r="J79" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K79" s="1" t="s">
         <v>69</v>
@@ -4810,11 +4810,11 @@
       </c>
       <c r="E80" s="1">
         <f ca="1">dates!$B$3+D80-1</f>
-        <v>44317</v>
+        <v>44348</v>
       </c>
       <c r="G80" s="1">
         <f ca="1">E80+7-1</f>
-        <v>44323</v>
+        <v>44354</v>
       </c>
       <c r="H80" s="1" t="b">
         <f ca="1">OR(E80&lt;dates!$B$3,E80&gt;dates!$B$4)</f>
@@ -4824,8 +4824,8 @@
         <v>8</v>
       </c>
       <c r="J80" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
@@ -4843,14 +4843,14 @@
       </c>
       <c r="E81" s="1">
         <f ca="1">dates!$B$3+D81-1</f>
-        <v>44326</v>
+        <v>44357</v>
       </c>
       <c r="F81" s="16">
         <v>7</v>
       </c>
       <c r="G81" s="1">
         <f ca="1">E81+7</f>
-        <v>44333</v>
+        <v>44364</v>
       </c>
       <c r="H81" s="1" t="b">
         <f ca="1">OR(E81&lt;dates!$B$3,E81&gt;dates!$B$4)</f>
@@ -4860,8 +4860,8 @@
         <v>8</v>
       </c>
       <c r="J81" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
@@ -4879,14 +4879,14 @@
       </c>
       <c r="E82" s="1">
         <f ca="1">dates!$B$3+D82-1</f>
-        <v>44331</v>
+        <v>44362</v>
       </c>
       <c r="F82" s="16">
         <v>15</v>
       </c>
       <c r="G82" s="1">
         <f ca="1">IF(F82&gt;=D82,dates!$B$3+F82-1,dates!$B$6+F82-1)</f>
-        <v>44331</v>
+        <v>44362</v>
       </c>
       <c r="H82" s="1" t="b">
         <f ca="1">OR(E82&lt;dates!$B$3,E82&gt;dates!$B$4)</f>
@@ -4896,8 +4896,8 @@
         <v>8</v>
       </c>
       <c r="J82" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K82" s="1" t="s">
         <v>69</v>
@@ -4922,14 +4922,14 @@
       </c>
       <c r="E83" s="1">
         <f ca="1">dates!$B$3+D83-1</f>
-        <v>44331</v>
+        <v>44362</v>
       </c>
       <c r="F83" s="16">
         <v>15</v>
       </c>
       <c r="G83" s="1">
         <f ca="1">IF(F83&gt;=D83,dates!$B$3+F83-1,dates!$B$6+F83-1)</f>
-        <v>44331</v>
+        <v>44362</v>
       </c>
       <c r="H83" s="1" t="b">
         <f ca="1">OR(E83&lt;dates!$B$3,E83&gt;dates!$B$4)</f>
@@ -4939,8 +4939,8 @@
         <v>8</v>
       </c>
       <c r="J83" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K83" s="1" t="s">
         <v>69</v>
@@ -4962,18 +4962,18 @@
       </c>
       <c r="D84">
         <f ca="1">DAY(dates!$B$4)</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E84" s="1">
         <f ca="1">dates!$B$4</f>
-        <v>44347</v>
+        <v>44377</v>
       </c>
       <c r="F84" s="16">
         <v>7</v>
       </c>
       <c r="G84" s="19">
         <f ca="1">E84+7</f>
-        <v>44354</v>
+        <v>44384</v>
       </c>
       <c r="H84" s="1" t="b">
         <f ca="1">OR(E84&lt;dates!$B$3,E84&gt;dates!$B$4)</f>
@@ -4983,8 +4983,8 @@
         <v>8</v>
       </c>
       <c r="J84" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K84" s="1" t="s">
         <v>75</v>
@@ -5006,18 +5006,18 @@
       </c>
       <c r="D85">
         <f ca="1">DAY(dates!$B$4)</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E85" s="1">
         <f ca="1">dates!$B$4</f>
-        <v>44347</v>
+        <v>44377</v>
       </c>
       <c r="F85" s="16">
         <v>7</v>
       </c>
       <c r="G85" s="19">
         <f ca="1">E85+7</f>
-        <v>44354</v>
+        <v>44384</v>
       </c>
       <c r="H85" s="1" t="b">
         <f ca="1">OR(E85&lt;dates!$B$3,E85&gt;dates!$B$4)</f>
@@ -5027,8 +5027,8 @@
         <v>8</v>
       </c>
       <c r="J85" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K85" s="1" t="s">
         <v>75</v>
@@ -5053,11 +5053,11 @@
       </c>
       <c r="E86" s="1">
         <f ca="1">dates!$B$3+D86-1</f>
-        <v>44317</v>
+        <v>44348</v>
       </c>
       <c r="G86" s="1">
         <f ca="1">E86+7-1</f>
-        <v>44323</v>
+        <v>44354</v>
       </c>
       <c r="H86" s="1" t="b">
         <f ca="1">OR(E86&lt;dates!$B$3,E86&gt;dates!$B$4)</f>
@@ -5067,8 +5067,8 @@
         <v>8</v>
       </c>
       <c r="J86" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L86" s="1"/>
     </row>
@@ -5087,14 +5087,14 @@
       </c>
       <c r="E87" s="1">
         <f ca="1">dates!$B$3+D87-1</f>
-        <v>44317</v>
+        <v>44348</v>
       </c>
       <c r="F87" s="16">
         <v>7</v>
       </c>
       <c r="G87" s="1">
         <f ca="1">E87+7</f>
-        <v>44324</v>
+        <v>44355</v>
       </c>
       <c r="H87" s="1" t="b">
         <f ca="1">OR(E87&lt;dates!$B$3,E87&gt;dates!$B$4)</f>
@@ -5104,8 +5104,8 @@
         <v>8</v>
       </c>
       <c r="J87" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L87" s="1"/>
     </row>
@@ -5124,11 +5124,11 @@
       </c>
       <c r="E88" s="1">
         <f ca="1">dates!$B$3+D88-1</f>
-        <v>44332</v>
+        <v>44363</v>
       </c>
       <c r="G88" s="1">
         <f ca="1">E88+7</f>
-        <v>44339</v>
+        <v>44370</v>
       </c>
       <c r="H88" s="1" t="b">
         <f ca="1">OR(E88&lt;dates!$B$3,E88&gt;dates!$B$4)</f>
@@ -5138,8 +5138,8 @@
         <v>8</v>
       </c>
       <c r="J88" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L88" s="1"/>
     </row>
@@ -5158,11 +5158,11 @@
       </c>
       <c r="E89" s="1">
         <f ca="1">dates!$B$3+D89-1</f>
-        <v>44332</v>
+        <v>44363</v>
       </c>
       <c r="G89" s="1">
         <f ca="1">E89+7</f>
-        <v>44339</v>
+        <v>44370</v>
       </c>
       <c r="H89" s="1" t="b">
         <f ca="1">OR(E89&lt;dates!$B$3,E89&gt;dates!$B$4)</f>
@@ -5172,8 +5172,8 @@
         <v>8</v>
       </c>
       <c r="J89" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L89" s="1"/>
     </row>
@@ -5192,14 +5192,14 @@
       </c>
       <c r="E90" s="1">
         <f ca="1">dates!$B$3+D90-1</f>
-        <v>44324</v>
+        <v>44355</v>
       </c>
       <c r="F90" s="16">
         <v>8</v>
       </c>
       <c r="G90" s="1">
         <f ca="1">IF(F90&gt;=D90,dates!$B$3+F90-1,dates!$B$6+F90-1)</f>
-        <v>44324</v>
+        <v>44355</v>
       </c>
       <c r="H90" s="1" t="b">
         <f ca="1">OR(E90&lt;dates!$B$3,E90&gt;dates!$B$4)</f>
@@ -5209,8 +5209,8 @@
         <v>8</v>
       </c>
       <c r="J90" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K90" s="1" t="s">
         <v>71</v>
@@ -5235,11 +5235,11 @@
       </c>
       <c r="E91" s="1">
         <f ca="1">dates!$B$3+D91-1</f>
-        <v>44332</v>
+        <v>44363</v>
       </c>
       <c r="G91" s="1">
         <f ca="1">E91+7</f>
-        <v>44339</v>
+        <v>44370</v>
       </c>
       <c r="H91" s="1" t="b">
         <f ca="1">OR(E91&lt;dates!$B$3,E91&gt;dates!$B$4)</f>
@@ -5249,8 +5249,8 @@
         <v>8</v>
       </c>
       <c r="J91" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L91" s="1"/>
     </row>
@@ -5269,11 +5269,11 @@
       </c>
       <c r="E92" s="1">
         <f ca="1">dates!$B$3+D92-1</f>
-        <v>44317</v>
+        <v>44348</v>
       </c>
       <c r="G92" s="1">
         <f ca="1">E92+7</f>
-        <v>44324</v>
+        <v>44355</v>
       </c>
       <c r="H92" s="1" t="b">
         <f ca="1">OR(E92&lt;dates!$B$3,E92&gt;dates!$B$4)</f>
@@ -5283,8 +5283,8 @@
         <v>8</v>
       </c>
       <c r="J92" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L92" s="1"/>
     </row>
@@ -5303,7 +5303,7 @@
       </c>
       <c r="E93" s="1">
         <f ca="1">dates!$B$3+D93-1</f>
-        <v>44332</v>
+        <v>44363</v>
       </c>
       <c r="F93" s="16">
         <f>D93+7</f>
@@ -5311,7 +5311,7 @@
       </c>
       <c r="G93" s="19">
         <f ca="1">E93+7</f>
-        <v>44339</v>
+        <v>44370</v>
       </c>
       <c r="H93" s="1" t="b">
         <f ca="1">OR(E93&lt;dates!$B$3,E93&gt;dates!$B$4)</f>
@@ -5321,8 +5321,8 @@
         <v>8</v>
       </c>
       <c r="J93" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K93" s="1" t="s">
         <v>73</v>
@@ -5344,18 +5344,18 @@
       </c>
       <c r="D94">
         <f ca="1">DAY(dates!$B$4)</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E94" s="1">
         <f ca="1">dates!$B$3+D94-1</f>
-        <v>44347</v>
+        <v>44377</v>
       </c>
       <c r="F94" s="16">
         <v>7</v>
       </c>
       <c r="G94" s="19">
         <f ca="1">dates!$B$4+7</f>
-        <v>44354</v>
+        <v>44384</v>
       </c>
       <c r="H94" s="1" t="b">
         <f ca="1">OR(E94&lt;dates!$B$3,E94&gt;dates!$B$4)</f>
@@ -5365,8 +5365,8 @@
         <v>8</v>
       </c>
       <c r="J94" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K94" s="1" t="s">
         <v>73</v>
@@ -5391,14 +5391,14 @@
       </c>
       <c r="E95" s="1">
         <f ca="1">dates!$B$3+D95-1</f>
-        <v>44331</v>
+        <v>44362</v>
       </c>
       <c r="F95" s="16">
         <v>11</v>
       </c>
       <c r="G95" s="1">
         <f ca="1">IF(F95&gt;=D95,dates!$B$3+F95-1,dates!$B$6+F95-1)</f>
-        <v>44358</v>
+        <v>44388</v>
       </c>
       <c r="H95" s="1" t="b">
         <f ca="1">OR(E95&lt;dates!$B$3,E95&gt;dates!$B$4)</f>
@@ -5408,8 +5408,8 @@
         <v>8</v>
       </c>
       <c r="J95" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K95" s="1" t="s">
         <v>69</v>
@@ -5434,11 +5434,11 @@
       </c>
       <c r="E96" s="1">
         <f ca="1">dates!$B$3+D96-1</f>
-        <v>44331</v>
+        <v>44362</v>
       </c>
       <c r="G96" s="1">
         <f ca="1">E96+7</f>
-        <v>44338</v>
+        <v>44369</v>
       </c>
       <c r="H96" s="1" t="b">
         <f ca="1">OR(E96&lt;dates!$B$3,E96&gt;dates!$B$4)</f>
@@ -5448,8 +5448,8 @@
         <v>8</v>
       </c>
       <c r="J96" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L96" s="1"/>
     </row>
@@ -5468,11 +5468,11 @@
       </c>
       <c r="E97" s="1">
         <f ca="1">dates!$B$3+D97-1</f>
-        <v>44331</v>
+        <v>44362</v>
       </c>
       <c r="G97" s="1">
         <f ca="1">E97+7</f>
-        <v>44338</v>
+        <v>44369</v>
       </c>
       <c r="H97" s="1" t="b">
         <f ca="1">OR(E97&lt;dates!$B$3,E97&gt;dates!$B$4)</f>
@@ -5482,8 +5482,8 @@
         <v>8</v>
       </c>
       <c r="J97" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="L97" s="1"/>
     </row>
@@ -5519,8 +5519,8 @@
         <v>8</v>
       </c>
       <c r="J98" s="1">
-        <f ca="1">NOW()</f>
-        <v>44316.710979398151</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44319.453377314814</v>
       </c>
       <c r="K98" s="1" t="s">
         <v>71</v>
@@ -5581,11 +5581,11 @@
       </c>
       <c r="B2" s="1">
         <f ca="1">EOMONTH(NOW(),0)</f>
-        <v>44316</v>
+        <v>44347</v>
       </c>
       <c r="E2" s="1">
         <f ca="1">EOMONTH(NOW(),0)</f>
-        <v>44316</v>
+        <v>44347</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -5594,7 +5594,7 @@
       </c>
       <c r="B3" s="1">
         <f ca="1">EOMONTH(B2,0)+1</f>
-        <v>44317</v>
+        <v>44348</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -5603,7 +5603,7 @@
       </c>
       <c r="B4" s="1">
         <f ca="1">EOMONTH(B2,1)</f>
-        <v>44347</v>
+        <v>44377</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -5612,7 +5612,7 @@
       </c>
       <c r="B5" s="1">
         <f ca="1">_xlfn.CEILING.MATH((B3+B4)/2,1)</f>
-        <v>44332</v>
+        <v>44363</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -5621,7 +5621,7 @@
       </c>
       <c r="B6" s="1">
         <f ca="1">B4+1</f>
-        <v>44348</v>
+        <v>44378</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5630,7 +5630,7 @@
       </c>
       <c r="B7" s="1">
         <f ca="1">DATE(YEAR($B$3),MONTH($B$3),'Which Week'!B8)-WEEKDAY(DATE(YEAR($B$3),MONTH($B$3),'Day of Week'!$B$11))</f>
-        <v>44321</v>
+        <v>44349</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5639,7 +5639,7 @@
       </c>
       <c r="B8" s="1">
         <f ca="1">DATE(YEAR($B$3),MONTH($B$3),'Which Week'!B9)-WEEKDAY(DATE(YEAR($B$3),MONTH($B$3),'Day of Week'!$B$11))</f>
-        <v>44328</v>
+        <v>44356</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5648,7 +5648,7 @@
       </c>
       <c r="B9" s="1">
         <f ca="1">DATE(YEAR($B$3),MONTH($B$3),'Which Week'!B10)-WEEKDAY(DATE(YEAR($B$3),MONTH($B$3),'Day of Week'!$B$11))</f>
-        <v>44335</v>
+        <v>44363</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5657,16 +5657,16 @@
       </c>
       <c r="B10" s="1">
         <f ca="1">DATE(YEAR($B$3),MONTH($B$3),'Which Week'!B11)-WEEKDAY(DATE(YEAR($B$3),MONTH($B$3),'Day of Week'!$B$11))</f>
-        <v>44342</v>
+        <v>44370</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="1" t="e">
+      <c r="B11" s="1">
         <f ca="1">IF(MONTH(DATE(YEAR($B$3),MONTH($B$3),'Which Week'!B12)-WEEKDAY(DATE(YEAR($B$3),MONTH($B$3),'Day of Week'!$B$11)))=MONTH(B10),DATE(YEAR($B$3),MONTH($B$3),'Which Week'!B12)-WEEKDAY(DATE(YEAR($B$3),MONTH($B$3),'Day of Week'!$B$11)),NA())</f>
-        <v>#N/A</v>
+        <v>44377</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed. #34 Update TD Ameritrade Download Start Date to day 03.
</commit_message>
<xml_diff>
--- a/var/skuld-base.xlsx
+++ b/var/skuld-base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\J70397102-skuld\var\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB710BC-27BB-4937-AEB4-8C84CC1503E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D164E6-696D-406D-B6C9-07ECA81DCC75}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1260" yWindow="1650" windowWidth="21000" windowHeight="13530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1639,10 +1639,10 @@
   <dimension ref="A1:M98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
+      <selection pane="bottomRight" activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1730,7 +1730,7 @@
       </c>
       <c r="J2" s="1">
         <f t="shared" ref="J2:J33" ca="1" si="0">NOW()</f>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>73</v>
@@ -1770,7 +1770,7 @@
       </c>
       <c r="J3" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L3" s="1"/>
     </row>
@@ -1804,7 +1804,7 @@
       </c>
       <c r="J4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L4" s="1"/>
     </row>
@@ -1841,7 +1841,7 @@
       </c>
       <c r="J5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>69</v>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="J6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L6" s="1"/>
     </row>
@@ -1915,7 +1915,7 @@
       </c>
       <c r="J7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L7" s="1"/>
     </row>
@@ -1949,7 +1949,7 @@
       </c>
       <c r="J8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L8" s="1"/>
     </row>
@@ -1986,7 +1986,7 @@
       </c>
       <c r="J9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>69</v>
@@ -2026,7 +2026,7 @@
       </c>
       <c r="J10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L10" s="1"/>
     </row>
@@ -2063,7 +2063,7 @@
       </c>
       <c r="J11" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K11" s="19" t="s">
         <v>71</v>
@@ -2109,7 +2109,7 @@
       </c>
       <c r="J12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>71</v>
@@ -2152,7 +2152,7 @@
       </c>
       <c r="J13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>69</v>
@@ -2192,7 +2192,7 @@
       </c>
       <c r="J14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L14" s="1"/>
     </row>
@@ -2226,7 +2226,7 @@
       </c>
       <c r="J15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L15" s="1"/>
     </row>
@@ -2263,7 +2263,7 @@
       </c>
       <c r="J16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>69</v>
@@ -2303,7 +2303,7 @@
       </c>
       <c r="J17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L17" s="1"/>
     </row>
@@ -2337,7 +2337,7 @@
       </c>
       <c r="J18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L18" s="1"/>
     </row>
@@ -2376,7 +2376,7 @@
       </c>
       <c r="J19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L19" t="s">
         <v>121</v>
@@ -2416,7 +2416,7 @@
       </c>
       <c r="J20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>74</v>
@@ -2458,7 +2458,7 @@
       </c>
       <c r="J21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -2494,7 +2494,7 @@
       </c>
       <c r="J22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L22" s="1"/>
     </row>
@@ -2532,7 +2532,7 @@
       </c>
       <c r="J23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>74</v>
@@ -2574,7 +2574,7 @@
       </c>
       <c r="J24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -2611,7 +2611,7 @@
       </c>
       <c r="J25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -2650,7 +2650,7 @@
       </c>
       <c r="J26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>69</v>
@@ -2694,7 +2694,7 @@
       </c>
       <c r="J27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L27" s="1"/>
     </row>
@@ -2728,7 +2728,7 @@
       </c>
       <c r="J28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L28" s="1"/>
     </row>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="J29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>71</v>
@@ -2811,7 +2811,7 @@
       </c>
       <c r="J30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>69</v>
@@ -2851,7 +2851,7 @@
       </c>
       <c r="J31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L31" s="1"/>
     </row>
@@ -2885,7 +2885,7 @@
       </c>
       <c r="J32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L32" s="1"/>
     </row>
@@ -2922,7 +2922,7 @@
       </c>
       <c r="J33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L33" s="1" t="str">
         <f>"S/S: "&amp;K33</f>
@@ -2965,7 +2965,7 @@
       </c>
       <c r="J34" s="1">
         <f t="shared" ref="J34:J65" ca="1" si="1">NOW()</f>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>69</v>
@@ -3005,7 +3005,7 @@
       </c>
       <c r="J35" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L35" s="1"/>
     </row>
@@ -3039,7 +3039,7 @@
       </c>
       <c r="J36" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L36" s="1"/>
     </row>
@@ -3076,7 +3076,7 @@
       </c>
       <c r="J37" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>76</v>
@@ -3122,7 +3122,7 @@
       </c>
       <c r="J38" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>69</v>
@@ -3165,7 +3165,7 @@
       </c>
       <c r="J39" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>69</v>
@@ -3208,7 +3208,7 @@
       </c>
       <c r="J40" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>69</v>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="J41" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="M41">
         <v>1</v>
@@ -3290,7 +3290,7 @@
       </c>
       <c r="J42" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>69</v>
@@ -3336,7 +3336,7 @@
       </c>
       <c r="J43" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>71</v>
@@ -3379,7 +3379,7 @@
       </c>
       <c r="J44" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>71</v>
@@ -3422,7 +3422,7 @@
       </c>
       <c r="J45" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>71</v>
@@ -3466,7 +3466,7 @@
       </c>
       <c r="J46" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K46" s="1" t="s">
         <v>71</v>
@@ -3512,7 +3512,7 @@
       </c>
       <c r="J47" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>71</v>
@@ -3554,7 +3554,7 @@
       </c>
       <c r="J48" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K48" s="1" t="s">
         <v>71</v>
@@ -3600,7 +3600,7 @@
       </c>
       <c r="J49" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K49" s="1" t="s">
         <v>69</v>
@@ -3646,7 +3646,7 @@
       </c>
       <c r="J50" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>69</v>
@@ -3692,7 +3692,7 @@
       </c>
       <c r="J51" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K51" s="1" t="s">
         <v>69</v>
@@ -3732,7 +3732,7 @@
       </c>
       <c r="J52" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L52" s="1"/>
     </row>
@@ -3766,7 +3766,7 @@
       </c>
       <c r="J53" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L53" s="1"/>
     </row>
@@ -3803,7 +3803,7 @@
       </c>
       <c r="J54" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>76</v>
@@ -3846,7 +3846,7 @@
       </c>
       <c r="J55" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
@@ -3882,7 +3882,7 @@
       </c>
       <c r="J56" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
@@ -3918,7 +3918,7 @@
       </c>
       <c r="J57" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -3955,7 +3955,7 @@
       </c>
       <c r="J58" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K58" s="19" t="s">
         <v>69</v>
@@ -3997,7 +3997,7 @@
       </c>
       <c r="J59" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K59" s="19"/>
       <c r="L59" s="19"/>
@@ -4034,7 +4034,7 @@
       </c>
       <c r="J60" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K60" s="19"/>
       <c r="L60" s="19"/>
@@ -4073,7 +4073,7 @@
       </c>
       <c r="J61" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
@@ -4109,7 +4109,7 @@
       </c>
       <c r="J62" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
@@ -4145,7 +4145,7 @@
       </c>
       <c r="J63" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
@@ -4181,7 +4181,7 @@
       </c>
       <c r="J64" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
@@ -4217,7 +4217,7 @@
       </c>
       <c r="J65" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
@@ -4253,7 +4253,7 @@
       </c>
       <c r="J66" s="1">
         <f t="shared" ref="J66:J98" ca="1" si="2">NOW()</f>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
@@ -4289,7 +4289,7 @@
       </c>
       <c r="J67" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
     </row>
     <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
@@ -4325,7 +4325,7 @@
       </c>
       <c r="J68" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K68" s="19" t="s">
         <v>69</v>
@@ -4371,7 +4371,7 @@
       </c>
       <c r="J69" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K69" s="1" t="s">
         <v>77</v>
@@ -4414,7 +4414,7 @@
       </c>
       <c r="J70" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K70" s="1" t="s">
         <v>69</v>
@@ -4454,7 +4454,7 @@
       </c>
       <c r="J71" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L71" s="1"/>
     </row>
@@ -4488,7 +4488,7 @@
       </c>
       <c r="J72" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L72" s="1"/>
     </row>
@@ -4525,7 +4525,7 @@
       </c>
       <c r="J73" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K73" s="1" t="s">
         <v>71</v>
@@ -4569,7 +4569,7 @@
       </c>
       <c r="J74" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K74" s="1" t="s">
         <v>70</v>
@@ -4613,7 +4613,7 @@
       </c>
       <c r="J75" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K75" s="1" t="s">
         <v>70</v>
@@ -4657,7 +4657,7 @@
       </c>
       <c r="J76" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K76" s="1" t="s">
         <v>71</v>
@@ -4700,7 +4700,7 @@
       </c>
       <c r="J77" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K77" s="1" t="s">
         <v>71</v>
@@ -4742,7 +4742,7 @@
       </c>
       <c r="J78" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K78" s="1" t="s">
         <v>69</v>
@@ -4785,7 +4785,7 @@
       </c>
       <c r="J79" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K79" s="1" t="s">
         <v>69</v>
@@ -4806,15 +4806,15 @@
         <v>9</v>
       </c>
       <c r="D80">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E80" s="1">
         <f ca="1">dates!$B$3+D80-1</f>
-        <v>44348</v>
+        <v>44350</v>
       </c>
       <c r="G80" s="1">
         <f ca="1">E80+7-1</f>
-        <v>44354</v>
+        <v>44356</v>
       </c>
       <c r="H80" s="1" t="b">
         <f ca="1">OR(E80&lt;dates!$B$3,E80&gt;dates!$B$4)</f>
@@ -4825,7 +4825,7 @@
       </c>
       <c r="J80" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
@@ -4861,7 +4861,7 @@
       </c>
       <c r="J81" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
@@ -4897,7 +4897,7 @@
       </c>
       <c r="J82" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K82" s="1" t="s">
         <v>69</v>
@@ -4940,7 +4940,7 @@
       </c>
       <c r="J83" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K83" s="1" t="s">
         <v>69</v>
@@ -4984,7 +4984,7 @@
       </c>
       <c r="J84" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K84" s="1" t="s">
         <v>75</v>
@@ -5028,7 +5028,7 @@
       </c>
       <c r="J85" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K85" s="1" t="s">
         <v>75</v>
@@ -5068,7 +5068,7 @@
       </c>
       <c r="J86" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L86" s="1"/>
     </row>
@@ -5105,7 +5105,7 @@
       </c>
       <c r="J87" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L87" s="1"/>
     </row>
@@ -5139,7 +5139,7 @@
       </c>
       <c r="J88" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L88" s="1"/>
     </row>
@@ -5173,7 +5173,7 @@
       </c>
       <c r="J89" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L89" s="1"/>
     </row>
@@ -5210,7 +5210,7 @@
       </c>
       <c r="J90" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K90" s="1" t="s">
         <v>71</v>
@@ -5250,7 +5250,7 @@
       </c>
       <c r="J91" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L91" s="1"/>
     </row>
@@ -5284,7 +5284,7 @@
       </c>
       <c r="J92" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L92" s="1"/>
     </row>
@@ -5322,7 +5322,7 @@
       </c>
       <c r="J93" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K93" s="1" t="s">
         <v>73</v>
@@ -5366,7 +5366,7 @@
       </c>
       <c r="J94" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K94" s="1" t="s">
         <v>73</v>
@@ -5409,7 +5409,7 @@
       </c>
       <c r="J95" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K95" s="1" t="s">
         <v>69</v>
@@ -5449,7 +5449,7 @@
       </c>
       <c r="J96" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L96" s="1"/>
     </row>
@@ -5483,7 +5483,7 @@
       </c>
       <c r="J97" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="L97" s="1"/>
     </row>
@@ -5520,7 +5520,7 @@
       </c>
       <c r="J98" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.453377314814</v>
+        <v>44319.45838275463</v>
       </c>
       <c r="K98" s="1" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
Fixed. #35 Remove Texans Mark Tasks.
</commit_message>
<xml_diff>
--- a/var/skuld-base.xlsx
+++ b/var/skuld-base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\J70397102-skuld\var\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D164E6-696D-406D-B6C9-07ECA81DCC75}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3348B1-4BE6-4A64-A792-4BD5A7486CC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1260" yWindow="1650" windowWidth="21000" windowHeight="13530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="138">
   <si>
     <t>Task Name</t>
   </si>
@@ -595,9 +595,6 @@
     <t>Sears MC 5844</t>
   </si>
   <si>
-    <t>Texans MJJ Stmt</t>
-  </si>
-  <si>
     <t>Academy 6348</t>
   </si>
   <si>
@@ -686,9 +683,6 @@
   </si>
   <si>
     <t>FMOQ</t>
-  </si>
-  <si>
-    <t>Texans Mark Stmt</t>
   </si>
   <si>
     <t>Texans Marian Stmt</t>
@@ -1639,10 +1633,10 @@
   <dimension ref="A1:M98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B69" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D82" sqref="D82"/>
+      <selection pane="bottomRight" activeCell="A87" sqref="A87:XFD87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1679,7 +1673,7 @@
         <v>3</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>4</v>
@@ -1699,7 +1693,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -1730,7 +1724,7 @@
       </c>
       <c r="J2" s="1">
         <f t="shared" ref="J2:J33" ca="1" si="0">NOW()</f>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>73</v>
@@ -1742,7 +1736,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
         <v>88</v>
@@ -1770,13 +1764,13 @@
       </c>
       <c r="J3" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B4" t="s">
         <v>94</v>
@@ -1804,7 +1798,7 @@
       </c>
       <c r="J4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="L4" s="1"/>
     </row>
@@ -1841,7 +1835,7 @@
       </c>
       <c r="J5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>69</v>
@@ -1881,7 +1875,7 @@
       </c>
       <c r="J6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="L6" s="1"/>
     </row>
@@ -1915,13 +1909,13 @@
       </c>
       <c r="J7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B8" t="s">
         <v>88</v>
@@ -1949,13 +1943,13 @@
       </c>
       <c r="J8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -1986,7 +1980,7 @@
       </c>
       <c r="J9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>69</v>
@@ -1998,7 +1992,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B10" t="s">
         <v>94</v>
@@ -2026,7 +2020,7 @@
       </c>
       <c r="J10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="L10" s="1"/>
     </row>
@@ -2063,7 +2057,7 @@
       </c>
       <c r="J11" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K11" s="19" t="s">
         <v>71</v>
@@ -2109,7 +2103,7 @@
       </c>
       <c r="J12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>71</v>
@@ -2152,7 +2146,7 @@
       </c>
       <c r="J13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>69</v>
@@ -2192,7 +2186,7 @@
       </c>
       <c r="J14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="L14" s="1"/>
     </row>
@@ -2226,7 +2220,7 @@
       </c>
       <c r="J15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="L15" s="1"/>
     </row>
@@ -2263,7 +2257,7 @@
       </c>
       <c r="J16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>69</v>
@@ -2303,7 +2297,7 @@
       </c>
       <c r="J17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="L17" s="1"/>
     </row>
@@ -2337,16 +2331,16 @@
       </c>
       <c r="J18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
@@ -2376,15 +2370,15 @@
       </c>
       <c r="J19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="L19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
@@ -2416,7 +2410,7 @@
       </c>
       <c r="J20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>74</v>
@@ -2429,7 +2423,7 @@
     </row>
     <row r="21" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B21" t="s">
         <v>88</v>
@@ -2458,7 +2452,7 @@
       </c>
       <c r="J21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -2466,7 +2460,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B22" t="s">
         <v>94</v>
@@ -2494,13 +2488,13 @@
       </c>
       <c r="J22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="L22" s="1"/>
     </row>
     <row r="23" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B23" t="s">
         <v>19</v>
@@ -2532,7 +2526,7 @@
       </c>
       <c r="J23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>74</v>
@@ -2545,7 +2539,7 @@
     </row>
     <row r="24" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B24" t="s">
         <v>88</v>
@@ -2574,7 +2568,7 @@
       </c>
       <c r="J24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -2582,7 +2576,7 @@
     </row>
     <row r="25" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B25" t="s">
         <v>94</v>
@@ -2611,7 +2605,7 @@
       </c>
       <c r="J25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -2650,7 +2644,7 @@
       </c>
       <c r="J26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>69</v>
@@ -2694,7 +2688,7 @@
       </c>
       <c r="J27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="L27" s="1"/>
     </row>
@@ -2728,13 +2722,13 @@
       </c>
       <c r="J28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="L28" s="1"/>
     </row>
     <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B29" t="s">
         <v>37</v>
@@ -2765,7 +2759,7 @@
       </c>
       <c r="J29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>71</v>
@@ -2811,7 +2805,7 @@
       </c>
       <c r="J30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>69</v>
@@ -2851,7 +2845,7 @@
       </c>
       <c r="J31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="L31" s="1"/>
     </row>
@@ -2885,13 +2879,13 @@
       </c>
       <c r="J32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="L32" s="1"/>
     </row>
     <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B33" t="s">
         <v>37</v>
@@ -2922,7 +2916,7 @@
       </c>
       <c r="J33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="L33" s="1" t="str">
         <f>"S/S: "&amp;K33</f>
@@ -2965,7 +2959,7 @@
       </c>
       <c r="J34" s="1">
         <f t="shared" ref="J34:J65" ca="1" si="1">NOW()</f>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>69</v>
@@ -3005,7 +2999,7 @@
       </c>
       <c r="J35" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="L35" s="1"/>
     </row>
@@ -3039,7 +3033,7 @@
       </c>
       <c r="J36" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="L36" s="1"/>
     </row>
@@ -3076,7 +3070,7 @@
       </c>
       <c r="J37" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>76</v>
@@ -3122,7 +3116,7 @@
       </c>
       <c r="J38" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>69</v>
@@ -3165,7 +3159,7 @@
       </c>
       <c r="J39" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>69</v>
@@ -3208,7 +3202,7 @@
       </c>
       <c r="J40" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>69</v>
@@ -3251,7 +3245,7 @@
       </c>
       <c r="J41" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="M41">
         <v>1</v>
@@ -3290,7 +3284,7 @@
       </c>
       <c r="J42" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>69</v>
@@ -3305,7 +3299,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B43" t="s">
         <v>38</v>
@@ -3336,7 +3330,7 @@
       </c>
       <c r="J43" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>71</v>
@@ -3379,7 +3373,7 @@
       </c>
       <c r="J44" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>71</v>
@@ -3422,7 +3416,7 @@
       </c>
       <c r="J45" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>71</v>
@@ -3434,7 +3428,7 @@
     </row>
     <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B46" t="s">
         <v>37</v>
@@ -3466,7 +3460,7 @@
       </c>
       <c r="J46" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K46" s="1" t="s">
         <v>71</v>
@@ -3512,7 +3506,7 @@
       </c>
       <c r="J47" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>71</v>
@@ -3523,7 +3517,7 @@
     </row>
     <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B48" t="s">
         <v>37</v>
@@ -3554,7 +3548,7 @@
       </c>
       <c r="J48" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K48" s="1" t="s">
         <v>71</v>
@@ -3569,7 +3563,7 @@
     </row>
     <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B49" t="s">
         <v>37</v>
@@ -3600,7 +3594,7 @@
       </c>
       <c r="J49" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K49" s="1" t="s">
         <v>69</v>
@@ -3615,7 +3609,7 @@
     </row>
     <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B50" t="s">
         <v>37</v>
@@ -3646,7 +3640,7 @@
       </c>
       <c r="J50" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>69</v>
@@ -3692,7 +3686,7 @@
       </c>
       <c r="J51" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K51" s="1" t="s">
         <v>69</v>
@@ -3732,7 +3726,7 @@
       </c>
       <c r="J52" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="L52" s="1"/>
     </row>
@@ -3766,7 +3760,7 @@
       </c>
       <c r="J53" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="L53" s="1"/>
     </row>
@@ -3803,7 +3797,7 @@
       </c>
       <c r="J54" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>76</v>
@@ -3815,10 +3809,10 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B55" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C55" t="s">
         <v>9</v>
@@ -3846,15 +3840,15 @@
       </c>
       <c r="J55" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B56" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C56" t="s">
         <v>9</v>
@@ -3882,15 +3876,15 @@
       </c>
       <c r="J56" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B57" t="s">
         <v>104</v>
-      </c>
-      <c r="B57" t="s">
-        <v>105</v>
       </c>
       <c r="C57" t="s">
         <v>9</v>
@@ -3918,7 +3912,7 @@
       </c>
       <c r="J57" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -3955,7 +3949,7 @@
       </c>
       <c r="J58" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K58" s="19" t="s">
         <v>69</v>
@@ -3997,7 +3991,7 @@
       </c>
       <c r="J59" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K59" s="19"/>
       <c r="L59" s="19"/>
@@ -4034,7 +4028,7 @@
       </c>
       <c r="J60" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K60" s="19"/>
       <c r="L60" s="19"/>
@@ -4042,10 +4036,10 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B61" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C61" t="s">
         <v>9</v>
@@ -4073,15 +4067,15 @@
       </c>
       <c r="J61" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B62" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C62" t="s">
         <v>9</v>
@@ -4109,15 +4103,15 @@
       </c>
       <c r="J62" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B63" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C63" t="s">
         <v>9</v>
@@ -4145,15 +4139,15 @@
       </c>
       <c r="J63" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B64" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C64" t="s">
         <v>9</v>
@@ -4181,15 +4175,15 @@
       </c>
       <c r="J64" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B65" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C65" t="s">
         <v>9</v>
@@ -4217,15 +4211,15 @@
       </c>
       <c r="J65" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C66" t="s">
         <v>9</v>
@@ -4253,15 +4247,15 @@
       </c>
       <c r="J66" s="1">
         <f t="shared" ref="J66:J98" ca="1" si="2">NOW()</f>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B67" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C67" t="s">
         <v>9</v>
@@ -4289,7 +4283,7 @@
       </c>
       <c r="J67" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
     </row>
     <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
@@ -4325,7 +4319,7 @@
       </c>
       <c r="J68" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K68" s="19" t="s">
         <v>69</v>
@@ -4371,7 +4365,7 @@
       </c>
       <c r="J69" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K69" s="1" t="s">
         <v>77</v>
@@ -4414,7 +4408,7 @@
       </c>
       <c r="J70" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K70" s="1" t="s">
         <v>69</v>
@@ -4454,7 +4448,7 @@
       </c>
       <c r="J71" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="L71" s="1"/>
     </row>
@@ -4488,13 +4482,13 @@
       </c>
       <c r="J72" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="L72" s="1"/>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B73" t="s">
         <v>37</v>
@@ -4525,7 +4519,7 @@
       </c>
       <c r="J73" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K73" s="1" t="s">
         <v>71</v>
@@ -4569,7 +4563,7 @@
       </c>
       <c r="J74" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K74" s="1" t="s">
         <v>70</v>
@@ -4613,7 +4607,7 @@
       </c>
       <c r="J75" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K75" s="1" t="s">
         <v>70</v>
@@ -4657,7 +4651,7 @@
       </c>
       <c r="J76" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K76" s="1" t="s">
         <v>71</v>
@@ -4700,7 +4694,7 @@
       </c>
       <c r="J77" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K77" s="1" t="s">
         <v>71</v>
@@ -4742,7 +4736,7 @@
       </c>
       <c r="J78" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K78" s="1" t="s">
         <v>69</v>
@@ -4785,7 +4779,7 @@
       </c>
       <c r="J79" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K79" s="1" t="s">
         <v>69</v>
@@ -4797,7 +4791,7 @@
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B80" t="s">
         <v>88</v>
@@ -4825,12 +4819,12 @@
       </c>
       <c r="J80" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B81" t="s">
         <v>94</v>
@@ -4861,7 +4855,7 @@
       </c>
       <c r="J81" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
@@ -4897,7 +4891,7 @@
       </c>
       <c r="J82" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K82" s="1" t="s">
         <v>69</v>
@@ -4940,7 +4934,7 @@
       </c>
       <c r="J83" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K83" s="1" t="s">
         <v>69</v>
@@ -4952,7 +4946,7 @@
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B84" t="s">
         <v>19</v>
@@ -4984,7 +4978,7 @@
       </c>
       <c r="J84" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K84" s="1" t="s">
         <v>75</v>
@@ -4994,119 +4988,22 @@
         <v>S/S: TXCU</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B85" t="s">
-        <v>19</v>
-      </c>
-      <c r="C85" t="s">
-        <v>9</v>
-      </c>
-      <c r="D85">
-        <f ca="1">DAY(dates!$B$4)</f>
-        <v>30</v>
-      </c>
-      <c r="E85" s="1">
-        <f ca="1">dates!$B$4</f>
-        <v>44377</v>
-      </c>
-      <c r="F85" s="16">
-        <v>7</v>
-      </c>
-      <c r="G85" s="19">
-        <f ca="1">E85+7</f>
-        <v>44384</v>
-      </c>
-      <c r="H85" s="1" t="b">
-        <f ca="1">OR(E85&lt;dates!$B$3,E85&gt;dates!$B$4)</f>
-        <v>0</v>
-      </c>
-      <c r="I85" t="s">
-        <v>8</v>
-      </c>
-      <c r="J85" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
-      </c>
-      <c r="K85" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="L85" s="1" t="str">
-        <f>"S/S: "&amp;K85</f>
-        <v>S/S: TXCU</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B86" t="s">
-        <v>88</v>
-      </c>
-      <c r="C86" t="s">
-        <v>9</v>
-      </c>
-      <c r="D86">
-        <v>1</v>
-      </c>
-      <c r="E86" s="1">
-        <f ca="1">dates!$B$3+D86-1</f>
-        <v>44348</v>
-      </c>
-      <c r="G86" s="1">
-        <f ca="1">E86+7-1</f>
-        <v>44354</v>
-      </c>
-      <c r="H86" s="1" t="b">
-        <f ca="1">OR(E86&lt;dates!$B$3,E86&gt;dates!$B$4)</f>
-        <v>0</v>
-      </c>
-      <c r="I86" t="s">
-        <v>8</v>
-      </c>
-      <c r="J86" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
-      </c>
+    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E85" s="1"/>
+      <c r="G85" s="19"/>
+      <c r="H85" s="1"/>
+      <c r="L85" s="1"/>
+    </row>
+    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E86" s="1"/>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
       <c r="L86" s="1"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B87" t="s">
-        <v>94</v>
-      </c>
-      <c r="C87" t="s">
-        <v>9</v>
-      </c>
-      <c r="D87">
-        <v>1</v>
-      </c>
-      <c r="E87" s="1">
-        <f ca="1">dates!$B$3+D87-1</f>
-        <v>44348</v>
-      </c>
-      <c r="F87" s="16">
-        <v>7</v>
-      </c>
-      <c r="G87" s="1">
-        <f ca="1">E87+7</f>
-        <v>44355</v>
-      </c>
-      <c r="H87" s="1" t="b">
-        <f ca="1">OR(E87&lt;dates!$B$3,E87&gt;dates!$B$4)</f>
-        <v>0</v>
-      </c>
-      <c r="I87" t="s">
-        <v>8</v>
-      </c>
-      <c r="J87" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
-      </c>
+    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E87" s="1"/>
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
       <c r="L87" s="1"/>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
@@ -5139,7 +5036,7 @@
       </c>
       <c r="J88" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="L88" s="1"/>
     </row>
@@ -5173,7 +5070,7 @@
       </c>
       <c r="J89" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="L89" s="1"/>
     </row>
@@ -5210,7 +5107,7 @@
       </c>
       <c r="J90" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K90" s="1" t="s">
         <v>71</v>
@@ -5250,7 +5147,7 @@
       </c>
       <c r="J91" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="L91" s="1"/>
     </row>
@@ -5284,7 +5181,7 @@
       </c>
       <c r="J92" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="L92" s="1"/>
     </row>
@@ -5322,7 +5219,7 @@
       </c>
       <c r="J93" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K93" s="1" t="s">
         <v>73</v>
@@ -5366,7 +5263,7 @@
       </c>
       <c r="J94" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K94" s="1" t="s">
         <v>73</v>
@@ -5409,7 +5306,7 @@
       </c>
       <c r="J95" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K95" s="1" t="s">
         <v>69</v>
@@ -5449,7 +5346,7 @@
       </c>
       <c r="J96" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="L96" s="1"/>
     </row>
@@ -5483,7 +5380,7 @@
       </c>
       <c r="J97" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="L97" s="1"/>
     </row>
@@ -5520,7 +5417,7 @@
       </c>
       <c r="J98" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.45838275463</v>
+        <v>44319.463125694441</v>
       </c>
       <c r="K98" s="1" t="s">
         <v>71</v>
@@ -5671,7 +5568,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B12" s="1">
         <f ca="1">DATE(YEAR(B3),1,1)</f>
@@ -5680,7 +5577,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B13">
         <f ca="1">ROUNDUP(MONTH(B3)/3,0)</f>
@@ -5689,7 +5586,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B14" s="1">
         <f ca="1">DATE(YEAR(B12),(3*(B13-1)+1),1)</f>

</xml_diff>

<commit_message>
#32 Move Coastal Items to after the First of the Month.
</commit_message>
<xml_diff>
--- a/var/skuld-base.xlsx
+++ b/var/skuld-base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\J70397102-skuld\var\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3348B1-4BE6-4A64-A792-4BD5A7486CC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF16109F-AE65-484F-BE10-B63276F137A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="1650" windowWidth="21000" windowHeight="13530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21165" yWindow="2355" windowWidth="21000" windowHeight="13530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="skuld-20210501" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="136">
   <si>
     <t>Task Name</t>
   </si>
@@ -613,13 +613,7 @@
     <t>Process Mark's Response from Dr. Misaghian</t>
   </si>
   <si>
-    <t>Coastal Marian Statement</t>
-  </si>
-  <si>
     <t>Coastal Marian Stmt</t>
-  </si>
-  <si>
-    <t>Coastal Mark Statement</t>
   </si>
   <si>
     <t>Coastal Mark Stmt</t>
@@ -1633,10 +1627,10 @@
   <dimension ref="A1:M98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A87" sqref="A87:XFD87"/>
+      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1673,7 +1667,7 @@
         <v>3</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>4</v>
@@ -1724,7 +1718,7 @@
       </c>
       <c r="J2" s="1">
         <f t="shared" ref="J2:J33" ca="1" si="0">NOW()</f>
-        <v>44319.463125694441</v>
+        <v>44320.39575127315</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>73</v>
@@ -1764,7 +1758,7 @@
       </c>
       <c r="J3" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="L3" s="1"/>
     </row>
@@ -1798,7 +1792,7 @@
       </c>
       <c r="J4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="L4" s="1"/>
     </row>
@@ -1835,7 +1829,7 @@
       </c>
       <c r="J5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>69</v>
@@ -1875,7 +1869,7 @@
       </c>
       <c r="J6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="L6" s="1"/>
     </row>
@@ -1909,13 +1903,13 @@
       </c>
       <c r="J7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B8" t="s">
         <v>88</v>
@@ -1943,13 +1937,13 @@
       </c>
       <c r="J8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -1980,7 +1974,7 @@
       </c>
       <c r="J9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>69</v>
@@ -1992,7 +1986,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B10" t="s">
         <v>94</v>
@@ -2020,7 +2014,7 @@
       </c>
       <c r="J10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="L10" s="1"/>
     </row>
@@ -2057,7 +2051,7 @@
       </c>
       <c r="J11" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K11" s="19" t="s">
         <v>71</v>
@@ -2103,7 +2097,7 @@
       </c>
       <c r="J12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>71</v>
@@ -2146,7 +2140,7 @@
       </c>
       <c r="J13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>69</v>
@@ -2186,7 +2180,7 @@
       </c>
       <c r="J14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="L14" s="1"/>
     </row>
@@ -2220,7 +2214,7 @@
       </c>
       <c r="J15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="L15" s="1"/>
     </row>
@@ -2257,7 +2251,7 @@
       </c>
       <c r="J16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>69</v>
@@ -2297,7 +2291,7 @@
       </c>
       <c r="J17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="L17" s="1"/>
     </row>
@@ -2331,16 +2325,16 @@
       </c>
       <c r="J18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B19" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
@@ -2370,10 +2364,10 @@
       </c>
       <c r="J19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="L19" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2395,11 +2389,11 @@
         <v>44377</v>
       </c>
       <c r="F20" s="16">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="G20" s="1">
         <f ca="1">IF(F20&gt;=D20,dates!$B$3+F20-1,dates!$B$6+F20-1)</f>
-        <v>44384</v>
+        <v>44377</v>
       </c>
       <c r="H20" s="1" t="b">
         <f ca="1">OR(E20&lt;dates!$B$3,E20&gt;dates!$B$4)</f>
@@ -2410,7 +2404,7 @@
       </c>
       <c r="J20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>74</v>
@@ -2423,7 +2417,7 @@
     </row>
     <row r="21" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B21" t="s">
         <v>88</v>
@@ -2432,16 +2426,18 @@
         <v>9</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E21" s="1">
         <f ca="1">dates!$B$3+D21-1</f>
-        <v>44348</v>
-      </c>
-      <c r="F21" s="16"/>
+        <v>44351</v>
+      </c>
+      <c r="F21" s="16">
+        <v>7</v>
+      </c>
       <c r="G21" s="1">
         <f ca="1">E21+7</f>
-        <v>44355</v>
+        <v>44358</v>
       </c>
       <c r="H21" s="1" t="b">
         <f ca="1">OR(E21&lt;dates!$B$3,E21&gt;dates!$B$4)</f>
@@ -2452,7 +2448,7 @@
       </c>
       <c r="J21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -2460,7 +2456,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B22" t="s">
         <v>94</v>
@@ -2469,15 +2465,18 @@
         <v>9</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E22" s="1">
         <f ca="1">dates!$B$3+D22-1</f>
-        <v>44348</v>
+        <v>44351</v>
+      </c>
+      <c r="F22" s="16">
+        <v>12</v>
       </c>
       <c r="G22" s="1">
         <f ca="1">E22+7</f>
-        <v>44355</v>
+        <v>44358</v>
       </c>
       <c r="H22" s="1" t="b">
         <f ca="1">OR(E22&lt;dates!$B$3,E22&gt;dates!$B$4)</f>
@@ -2488,13 +2487,13 @@
       </c>
       <c r="J22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="L22" s="1"/>
     </row>
     <row r="23" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B23" t="s">
         <v>19</v>
@@ -2503,19 +2502,18 @@
         <v>9</v>
       </c>
       <c r="D23">
-        <f ca="1">DAY(dates!$B$4)</f>
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="E23" s="1">
         <f ca="1">dates!$B$4</f>
         <v>44377</v>
       </c>
       <c r="F23" s="16">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="G23" s="1">
         <f ca="1">IF(F23&gt;=D23,dates!$B$3+F23-1,dates!$B$6+F23-1)</f>
-        <v>44384</v>
+        <v>44377</v>
       </c>
       <c r="H23" s="1" t="b">
         <f ca="1">OR(E23&lt;dates!$B$3,E23&gt;dates!$B$4)</f>
@@ -2526,7 +2524,7 @@
       </c>
       <c r="J23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>74</v>
@@ -2539,7 +2537,7 @@
     </row>
     <row r="24" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B24" t="s">
         <v>88</v>
@@ -2548,16 +2546,18 @@
         <v>9</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E24" s="1">
         <f ca="1">dates!$B$3+D24-1</f>
-        <v>44348</v>
-      </c>
-      <c r="F24" s="16"/>
+        <v>44351</v>
+      </c>
+      <c r="F24" s="16">
+        <v>7</v>
+      </c>
       <c r="G24" s="1">
         <f ca="1">E24+7</f>
-        <v>44355</v>
+        <v>44358</v>
       </c>
       <c r="H24" s="1" t="b">
         <f ca="1">OR(E24&lt;dates!$B$3,E24&gt;dates!$B$4)</f>
@@ -2568,7 +2568,7 @@
       </c>
       <c r="J24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -2576,7 +2576,7 @@
     </row>
     <row r="25" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B25" t="s">
         <v>94</v>
@@ -2585,16 +2585,18 @@
         <v>9</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E25" s="1">
         <f ca="1">dates!$B$3+D25-1</f>
-        <v>44348</v>
-      </c>
-      <c r="F25" s="16"/>
+        <v>44351</v>
+      </c>
+      <c r="F25" s="16">
+        <v>12</v>
+      </c>
       <c r="G25" s="1">
         <f ca="1">E25+7</f>
-        <v>44355</v>
+        <v>44358</v>
       </c>
       <c r="H25" s="1" t="b">
         <f ca="1">OR(E25&lt;dates!$B$3,E25&gt;dates!$B$4)</f>
@@ -2605,7 +2607,7 @@
       </c>
       <c r="J25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -2622,18 +2624,18 @@
         <v>9</v>
       </c>
       <c r="D26">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="E26" s="1">
         <f ca="1">dates!$B$3+D26-1</f>
-        <v>44375</v>
+        <v>44350</v>
       </c>
       <c r="F26" s="16">
         <v>23</v>
       </c>
       <c r="G26" s="1">
         <f ca="1">IF(F26&gt;=D26,dates!$B$3+F26-1,dates!$B$6+F26-1)</f>
-        <v>44400</v>
+        <v>44370</v>
       </c>
       <c r="H26" s="1" t="b">
         <f ca="1">OR(E26&lt;dates!$B$3,E26&gt;dates!$B$4)</f>
@@ -2644,7 +2646,7 @@
       </c>
       <c r="J26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>69</v>
@@ -2688,7 +2690,7 @@
       </c>
       <c r="J27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="L27" s="1"/>
     </row>
@@ -2703,15 +2705,18 @@
         <v>9</v>
       </c>
       <c r="D28">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="E28" s="1">
         <f ca="1">dates!$B$3+D28-1</f>
-        <v>44375</v>
+        <v>44350</v>
+      </c>
+      <c r="F28" s="16">
+        <v>12</v>
       </c>
       <c r="G28" s="1">
         <f ca="1">E28+7</f>
-        <v>44382</v>
+        <v>44357</v>
       </c>
       <c r="H28" s="1" t="b">
         <f ca="1">OR(E28&lt;dates!$B$3,E28&gt;dates!$B$4)</f>
@@ -2722,13 +2727,13 @@
       </c>
       <c r="J28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="L28" s="1"/>
     </row>
     <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B29" t="s">
         <v>37</v>
@@ -2759,7 +2764,7 @@
       </c>
       <c r="J29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>71</v>
@@ -2805,7 +2810,7 @@
       </c>
       <c r="J30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>69</v>
@@ -2845,7 +2850,7 @@
       </c>
       <c r="J31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="L31" s="1"/>
     </row>
@@ -2879,13 +2884,13 @@
       </c>
       <c r="J32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="L32" s="1"/>
     </row>
     <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B33" t="s">
         <v>37</v>
@@ -2916,7 +2921,7 @@
       </c>
       <c r="J33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="L33" s="1" t="str">
         <f>"S/S: "&amp;K33</f>
@@ -2959,7 +2964,7 @@
       </c>
       <c r="J34" s="1">
         <f t="shared" ref="J34:J65" ca="1" si="1">NOW()</f>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>69</v>
@@ -2999,7 +3004,7 @@
       </c>
       <c r="J35" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="L35" s="1"/>
     </row>
@@ -3033,7 +3038,7 @@
       </c>
       <c r="J36" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="L36" s="1"/>
     </row>
@@ -3070,7 +3075,7 @@
       </c>
       <c r="J37" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>76</v>
@@ -3116,7 +3121,7 @@
       </c>
       <c r="J38" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>69</v>
@@ -3159,7 +3164,7 @@
       </c>
       <c r="J39" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>69</v>
@@ -3202,7 +3207,7 @@
       </c>
       <c r="J40" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>69</v>
@@ -3245,7 +3250,7 @@
       </c>
       <c r="J41" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="M41">
         <v>1</v>
@@ -3284,7 +3289,7 @@
       </c>
       <c r="J42" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>69</v>
@@ -3299,7 +3304,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B43" t="s">
         <v>38</v>
@@ -3330,7 +3335,7 @@
       </c>
       <c r="J43" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>71</v>
@@ -3373,7 +3378,7 @@
       </c>
       <c r="J44" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>71</v>
@@ -3416,7 +3421,7 @@
       </c>
       <c r="J45" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>71</v>
@@ -3428,7 +3433,7 @@
     </row>
     <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B46" t="s">
         <v>37</v>
@@ -3460,7 +3465,7 @@
       </c>
       <c r="J46" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K46" s="1" t="s">
         <v>71</v>
@@ -3506,7 +3511,7 @@
       </c>
       <c r="J47" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>71</v>
@@ -3517,7 +3522,7 @@
     </row>
     <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B48" t="s">
         <v>37</v>
@@ -3548,7 +3553,7 @@
       </c>
       <c r="J48" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K48" s="1" t="s">
         <v>71</v>
@@ -3563,7 +3568,7 @@
     </row>
     <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B49" t="s">
         <v>37</v>
@@ -3594,7 +3599,7 @@
       </c>
       <c r="J49" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K49" s="1" t="s">
         <v>69</v>
@@ -3609,7 +3614,7 @@
     </row>
     <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B50" t="s">
         <v>37</v>
@@ -3640,7 +3645,7 @@
       </c>
       <c r="J50" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>69</v>
@@ -3686,7 +3691,7 @@
       </c>
       <c r="J51" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K51" s="1" t="s">
         <v>69</v>
@@ -3726,7 +3731,7 @@
       </c>
       <c r="J52" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="L52" s="1"/>
     </row>
@@ -3760,7 +3765,7 @@
       </c>
       <c r="J53" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="L53" s="1"/>
     </row>
@@ -3797,7 +3802,7 @@
       </c>
       <c r="J54" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>76</v>
@@ -3809,7 +3814,7 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B55" t="s">
         <v>104</v>
@@ -3840,12 +3845,12 @@
       </c>
       <c r="J55" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B56" t="s">
         <v>104</v>
@@ -3876,7 +3881,7 @@
       </c>
       <c r="J56" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
@@ -3912,7 +3917,7 @@
       </c>
       <c r="J57" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -3949,7 +3954,7 @@
       </c>
       <c r="J58" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K58" s="19" t="s">
         <v>69</v>
@@ -3991,7 +3996,7 @@
       </c>
       <c r="J59" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K59" s="19"/>
       <c r="L59" s="19"/>
@@ -4028,7 +4033,7 @@
       </c>
       <c r="J60" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K60" s="19"/>
       <c r="L60" s="19"/>
@@ -4036,7 +4041,7 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B61" t="s">
         <v>104</v>
@@ -4067,12 +4072,12 @@
       </c>
       <c r="J61" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B62" t="s">
         <v>104</v>
@@ -4103,7 +4108,7 @@
       </c>
       <c r="J62" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
@@ -4139,12 +4144,12 @@
       </c>
       <c r="J63" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B64" t="s">
         <v>104</v>
@@ -4175,7 +4180,7 @@
       </c>
       <c r="J64" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
@@ -4211,12 +4216,12 @@
       </c>
       <c r="J65" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B66" t="s">
         <v>104</v>
@@ -4247,7 +4252,7 @@
       </c>
       <c r="J66" s="1">
         <f t="shared" ref="J66:J98" ca="1" si="2">NOW()</f>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
@@ -4283,7 +4288,7 @@
       </c>
       <c r="J67" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
     </row>
     <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
@@ -4319,7 +4324,7 @@
       </c>
       <c r="J68" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K68" s="19" t="s">
         <v>69</v>
@@ -4365,7 +4370,7 @@
       </c>
       <c r="J69" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K69" s="1" t="s">
         <v>77</v>
@@ -4408,7 +4413,7 @@
       </c>
       <c r="J70" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K70" s="1" t="s">
         <v>69</v>
@@ -4448,7 +4453,7 @@
       </c>
       <c r="J71" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="L71" s="1"/>
     </row>
@@ -4482,13 +4487,13 @@
       </c>
       <c r="J72" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="L72" s="1"/>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B73" t="s">
         <v>37</v>
@@ -4519,7 +4524,7 @@
       </c>
       <c r="J73" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K73" s="1" t="s">
         <v>71</v>
@@ -4563,7 +4568,7 @@
       </c>
       <c r="J74" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K74" s="1" t="s">
         <v>70</v>
@@ -4607,7 +4612,7 @@
       </c>
       <c r="J75" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K75" s="1" t="s">
         <v>70</v>
@@ -4651,7 +4656,7 @@
       </c>
       <c r="J76" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K76" s="1" t="s">
         <v>71</v>
@@ -4694,7 +4699,7 @@
       </c>
       <c r="J77" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K77" s="1" t="s">
         <v>71</v>
@@ -4736,7 +4741,7 @@
       </c>
       <c r="J78" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K78" s="1" t="s">
         <v>69</v>
@@ -4779,7 +4784,7 @@
       </c>
       <c r="J79" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K79" s="1" t="s">
         <v>69</v>
@@ -4791,7 +4796,7 @@
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B80" t="s">
         <v>88</v>
@@ -4819,12 +4824,12 @@
       </c>
       <c r="J80" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B81" t="s">
         <v>94</v>
@@ -4855,7 +4860,7 @@
       </c>
       <c r="J81" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
@@ -4891,7 +4896,7 @@
       </c>
       <c r="J82" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K82" s="1" t="s">
         <v>69</v>
@@ -4934,7 +4939,7 @@
       </c>
       <c r="J83" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K83" s="1" t="s">
         <v>69</v>
@@ -4946,7 +4951,7 @@
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B84" t="s">
         <v>19</v>
@@ -4978,7 +4983,7 @@
       </c>
       <c r="J84" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K84" s="1" t="s">
         <v>75</v>
@@ -5036,7 +5041,7 @@
       </c>
       <c r="J88" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="L88" s="1"/>
     </row>
@@ -5070,7 +5075,7 @@
       </c>
       <c r="J89" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="L89" s="1"/>
     </row>
@@ -5107,7 +5112,7 @@
       </c>
       <c r="J90" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K90" s="1" t="s">
         <v>71</v>
@@ -5147,7 +5152,7 @@
       </c>
       <c r="J91" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="L91" s="1"/>
     </row>
@@ -5181,7 +5186,7 @@
       </c>
       <c r="J92" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="L92" s="1"/>
     </row>
@@ -5219,7 +5224,7 @@
       </c>
       <c r="J93" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K93" s="1" t="s">
         <v>73</v>
@@ -5263,7 +5268,7 @@
       </c>
       <c r="J94" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K94" s="1" t="s">
         <v>73</v>
@@ -5306,7 +5311,7 @@
       </c>
       <c r="J95" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K95" s="1" t="s">
         <v>69</v>
@@ -5346,7 +5351,7 @@
       </c>
       <c r="J96" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="L96" s="1"/>
     </row>
@@ -5380,7 +5385,7 @@
       </c>
       <c r="J97" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="L97" s="1"/>
     </row>
@@ -5417,7 +5422,7 @@
       </c>
       <c r="J98" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44319.463125694441</v>
+        <v>44320.395751157404</v>
       </c>
       <c r="K98" s="1" t="s">
         <v>71</v>
@@ -5568,7 +5573,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B12" s="1">
         <f ca="1">DATE(YEAR(B3),1,1)</f>
@@ -5577,7 +5582,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B13">
         <f ca="1">ROUNDUP(MONTH(B3)/3,0)</f>
@@ -5586,7 +5591,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B14" s="1">
         <f ca="1">DATE(YEAR(B12),(3*(B13-1)+1),1)</f>

</xml_diff>

<commit_message>
#28 All Banks Statements Should have Download Date about the First of the Month  #29 Add Edelman Performance Report Download  #30 Convert Lynda to Linked In Learning
</commit_message>
<xml_diff>
--- a/var/skuld-base.xlsx
+++ b/var/skuld-base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\J70397102-skuld\var\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF16109F-AE65-484F-BE10-B63276F137A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2101221A-B328-48CE-BA53-8795BDDA5DA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21165" yWindow="2355" windowWidth="21000" windowHeight="13530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2370" yWindow="150" windowWidth="21000" windowHeight="13530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="skuld-20210501" sheetId="1" r:id="rId1"/>
@@ -90,9 +90,6 @@
     <t>Google Pandora</t>
   </si>
   <si>
-    <t>Lynda</t>
-  </si>
-  <si>
     <t>Marine Federal Statement</t>
   </si>
   <si>
@@ -117,13 +114,7 @@
     <t>Spectrum</t>
   </si>
   <si>
-    <t>TD Americatrade Marian</t>
-  </si>
-  <si>
     <t>401(k) Distribution</t>
-  </si>
-  <si>
-    <t>TD Americatrade Mark</t>
   </si>
   <si>
     <t>USAA Insurance</t>
@@ -695,6 +686,15 @@
   </si>
   <si>
     <t>Contacts Plus</t>
+  </si>
+  <si>
+    <t>Edelman Marian (TDA)</t>
+  </si>
+  <si>
+    <t>Edelman Mark (TDA)</t>
+  </si>
+  <si>
+    <t>Linked In Learning (Lynda)</t>
   </si>
 </sst>
 </file>
@@ -1627,10 +1627,10 @@
   <dimension ref="A1:M98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomRight" activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1655,19 +1655,19 @@
         <v>5</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>4</v>
@@ -1676,18 +1676,18 @@
         <v>6</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -1718,10 +1718,10 @@
       </c>
       <c r="J2" s="1">
         <f t="shared" ref="J2:J33" ca="1" si="0">NOW()</f>
-        <v>44320.39575127315</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L2" s="1" t="str">
         <f>"S/S: "&amp;K2</f>
@@ -1730,10 +1730,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -1758,16 +1758,16 @@
       </c>
       <c r="J3" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -1792,13 +1792,13 @@
       </c>
       <c r="J4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -1829,10 +1829,10 @@
       </c>
       <c r="J5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L5" s="1" t="str">
         <f>"S/S: "&amp;K5</f>
@@ -1841,10 +1841,10 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -1869,16 +1869,16 @@
       </c>
       <c r="J6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -1903,16 +1903,16 @@
       </c>
       <c r="J7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -1937,13 +1937,13 @@
       </c>
       <c r="J8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -1974,10 +1974,10 @@
       </c>
       <c r="J9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L9" s="1" t="str">
         <f>"S/S: "&amp;K9</f>
@@ -1986,10 +1986,10 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
@@ -2014,19 +2014,19 @@
       </c>
       <c r="J10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:13" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D11" s="18">
         <v>1</v>
@@ -2051,10 +2051,10 @@
       </c>
       <c r="J11" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K11" s="19" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="L11" s="19" t="str">
         <f>"S/S: "&amp;K11</f>
@@ -2069,7 +2069,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
@@ -2097,10 +2097,10 @@
       </c>
       <c r="J12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="L12" s="1" t="str">
         <f>"S/S: "&amp;K12</f>
@@ -2109,7 +2109,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -2140,10 +2140,10 @@
       </c>
       <c r="J13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L13" s="1" t="str">
         <f>"S/S: "&amp;K13</f>
@@ -2152,10 +2152,10 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
@@ -2180,16 +2180,16 @@
       </c>
       <c r="J14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B15" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
@@ -2214,13 +2214,13 @@
       </c>
       <c r="J15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
@@ -2251,10 +2251,10 @@
       </c>
       <c r="J16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L16" s="1" t="str">
         <f>"S/S: "&amp;K16</f>
@@ -2263,10 +2263,10 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
@@ -2291,16 +2291,16 @@
       </c>
       <c r="J17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
@@ -2325,16 +2325,16 @@
       </c>
       <c r="J18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B19" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
@@ -2364,18 +2364,18 @@
       </c>
       <c r="J19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="L19" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
@@ -2404,10 +2404,10 @@
       </c>
       <c r="J20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="L20" s="1" t="str">
         <f>"S/S: "&amp;K20</f>
@@ -2417,10 +2417,10 @@
     </row>
     <row r="21" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B21" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
@@ -2448,7 +2448,7 @@
       </c>
       <c r="J21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -2456,10 +2456,10 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
@@ -2487,16 +2487,16 @@
       </c>
       <c r="J22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="L22" s="1"/>
     </row>
     <row r="23" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
@@ -2524,10 +2524,10 @@
       </c>
       <c r="J23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="L23" s="1" t="str">
         <f>"S/S: "&amp;K23</f>
@@ -2537,10 +2537,10 @@
     </row>
     <row r="24" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
@@ -2568,7 +2568,7 @@
       </c>
       <c r="J24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -2576,10 +2576,10 @@
     </row>
     <row r="25" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B25" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
@@ -2607,7 +2607,7 @@
       </c>
       <c r="J25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -2615,7 +2615,7 @@
     </row>
     <row r="26" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
@@ -2646,10 +2646,10 @@
       </c>
       <c r="J26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L26" s="1" t="str">
         <f>"S/S: "&amp;K26</f>
@@ -2659,10 +2659,10 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B27" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C27" t="s">
         <v>9</v>
@@ -2690,16 +2690,16 @@
       </c>
       <c r="J27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="L27" s="1"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B28" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C28" t="s">
         <v>9</v>
@@ -2727,19 +2727,19 @@
       </c>
       <c r="J28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="L28" s="1"/>
     </row>
     <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B29" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C29" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D29">
         <v>27</v>
@@ -2764,10 +2764,10 @@
       </c>
       <c r="J29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="L29" s="1" t="str">
         <f>"S/S: "&amp;K29</f>
@@ -2779,7 +2779,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B30" t="s">
         <v>7</v>
@@ -2810,10 +2810,10 @@
       </c>
       <c r="J30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L30" s="1" t="str">
         <f>"S/S: "&amp;K30</f>
@@ -2822,10 +2822,10 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C31" t="s">
         <v>9</v>
@@ -2850,16 +2850,16 @@
       </c>
       <c r="J31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="L31" s="1"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B32" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C32" t="s">
         <v>9</v>
@@ -2884,19 +2884,19 @@
       </c>
       <c r="J32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="L32" s="1"/>
     </row>
     <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -2921,7 +2921,7 @@
       </c>
       <c r="J33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="L33" s="1" t="str">
         <f>"S/S: "&amp;K33</f>
@@ -2933,7 +2933,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B34" t="s">
         <v>7</v>
@@ -2964,10 +2964,10 @@
       </c>
       <c r="J34" s="1">
         <f t="shared" ref="J34:J65" ca="1" si="1">NOW()</f>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L34" s="1" t="str">
         <f>"S/S: "&amp;K34</f>
@@ -2976,10 +2976,10 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B35" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C35" t="s">
         <v>9</v>
@@ -3004,16 +3004,16 @@
       </c>
       <c r="J35" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="L35" s="1"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B36" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C36" t="s">
         <v>9</v>
@@ -3038,19 +3038,19 @@
       </c>
       <c r="J36" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="L36" s="1"/>
     </row>
     <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C37" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -3075,10 +3075,10 @@
       </c>
       <c r="J37" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L37" s="1" t="str">
         <f>"S/S: "&amp;K37</f>
@@ -3090,10 +3090,10 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" t="s">
         <v>33</v>
-      </c>
-      <c r="B38" t="s">
-        <v>36</v>
       </c>
       <c r="C38" t="s">
         <v>9</v>
@@ -3121,10 +3121,10 @@
       </c>
       <c r="J38" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L38" s="1" t="str">
         <f>"S/S: "&amp;K38</f>
@@ -3164,10 +3164,10 @@
       </c>
       <c r="J39" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L39" s="1" t="str">
         <f>"S/S: "&amp;K39</f>
@@ -3207,10 +3207,10 @@
       </c>
       <c r="J40" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L40" s="1" t="str">
         <f>"S/S: "&amp;K40</f>
@@ -3219,13 +3219,13 @@
     </row>
     <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B41" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C41" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -3250,7 +3250,7 @@
       </c>
       <c r="J41" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="M41">
         <v>1</v>
@@ -3258,13 +3258,13 @@
     </row>
     <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B42" t="s">
         <v>10</v>
       </c>
       <c r="C42" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -3289,10 +3289,10 @@
       </c>
       <c r="J42" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L42" s="1" t="str">
         <f>"S/S: "&amp;K42</f>
@@ -3304,10 +3304,10 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B43" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C43" t="s">
         <v>9</v>
@@ -3335,10 +3335,10 @@
       </c>
       <c r="J43" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="L43" s="1" t="str">
         <f>"S/S: "&amp;K43</f>
@@ -3350,7 +3350,7 @@
         <v>15</v>
       </c>
       <c r="B44" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C44" t="s">
         <v>9</v>
@@ -3378,10 +3378,10 @@
       </c>
       <c r="J44" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="L44" s="1" t="str">
         <f>"S/S: "&amp;K44</f>
@@ -3393,7 +3393,7 @@
         <v>16</v>
       </c>
       <c r="B45" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C45" t="s">
         <v>9</v>
@@ -3421,10 +3421,10 @@
       </c>
       <c r="J45" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="L45" s="1" t="str">
         <f>"S/S: "&amp;K45</f>
@@ -3433,13 +3433,13 @@
     </row>
     <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B46" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C46" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D46">
         <f ca="1">DAY(E46)</f>
@@ -3465,10 +3465,10 @@
       </c>
       <c r="J46" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="L46" s="1" t="str">
         <f>"S/S: "&amp;K46</f>
@@ -3480,13 +3480,13 @@
     </row>
     <row r="47" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B47" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C47" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -3511,10 +3511,10 @@
       </c>
       <c r="J47" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="M47">
         <v>7</v>
@@ -3522,13 +3522,13 @@
     </row>
     <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B48" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C48" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D48">
         <v>20</v>
@@ -3553,10 +3553,10 @@
       </c>
       <c r="J48" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="L48" s="1" t="str">
         <f>"S/S: "&amp;K48</f>
@@ -3568,13 +3568,13 @@
     </row>
     <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B49" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C49" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -3599,10 +3599,10 @@
       </c>
       <c r="J49" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L49" s="1" t="str">
         <f>"S/S: "&amp;K49</f>
@@ -3614,13 +3614,13 @@
     </row>
     <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B50" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C50" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -3645,10 +3645,10 @@
       </c>
       <c r="J50" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L50" s="1" t="str">
         <f>"S/S: "&amp;K50</f>
@@ -3660,7 +3660,7 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B51" t="s">
         <v>7</v>
@@ -3691,10 +3691,10 @@
       </c>
       <c r="J51" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L51" s="1" t="str">
         <f>"S/S: "&amp;K51</f>
@@ -3703,10 +3703,10 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B52" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C52" t="s">
         <v>9</v>
@@ -3731,16 +3731,16 @@
       </c>
       <c r="J52" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="L52" s="1"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B53" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C53" t="s">
         <v>9</v>
@@ -3765,16 +3765,16 @@
       </c>
       <c r="J53" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="L53" s="1"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>17</v>
+        <v>135</v>
       </c>
       <c r="B54" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C54" t="s">
         <v>9</v>
@@ -3802,10 +3802,10 @@
       </c>
       <c r="J54" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L54" s="1" t="str">
         <f>"S/S: "&amp;K54</f>
@@ -3814,10 +3814,10 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B55" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C55" t="s">
         <v>9</v>
@@ -3845,15 +3845,15 @@
       </c>
       <c r="J55" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B56" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C56" t="s">
         <v>9</v>
@@ -3881,15 +3881,15 @@
       </c>
       <c r="J56" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B57" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C57" t="s">
         <v>9</v>
@@ -3917,15 +3917,15 @@
       </c>
       <c r="J57" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B58" s="18" t="s">
         <v>18</v>
-      </c>
-      <c r="B58" s="18" t="s">
-        <v>19</v>
       </c>
       <c r="C58" s="18" t="s">
         <v>9</v>
@@ -3954,10 +3954,10 @@
       </c>
       <c r="J58" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K58" s="19" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L58" s="19" t="str">
         <f>"S/S: "&amp;K58</f>
@@ -3967,10 +3967,10 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="17" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B59" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C59" s="18" t="s">
         <v>9</v>
@@ -3996,7 +3996,7 @@
       </c>
       <c r="J59" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K59" s="19"/>
       <c r="L59" s="19"/>
@@ -4004,10 +4004,10 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="17" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B60" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C60" s="18" t="s">
         <v>9</v>
@@ -4033,7 +4033,7 @@
       </c>
       <c r="J60" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K60" s="19"/>
       <c r="L60" s="19"/>
@@ -4041,10 +4041,10 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B61" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C61" t="s">
         <v>9</v>
@@ -4072,15 +4072,15 @@
       </c>
       <c r="J61" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B62" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C62" t="s">
         <v>9</v>
@@ -4108,15 +4108,15 @@
       </c>
       <c r="J62" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B63" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C63" t="s">
         <v>9</v>
@@ -4144,15 +4144,15 @@
       </c>
       <c r="J63" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B64" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C64" t="s">
         <v>9</v>
@@ -4180,15 +4180,15 @@
       </c>
       <c r="J64" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B65" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C65" t="s">
         <v>9</v>
@@ -4216,15 +4216,15 @@
       </c>
       <c r="J65" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B66" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C66" t="s">
         <v>9</v>
@@ -4252,15 +4252,15 @@
       </c>
       <c r="J66" s="1">
         <f t="shared" ref="J66:J98" ca="1" si="2">NOW()</f>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B67" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C67" t="s">
         <v>9</v>
@@ -4288,18 +4288,18 @@
       </c>
       <c r="J67" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
     </row>
     <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B68" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C68" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D68" s="18">
         <v>1</v>
@@ -4324,10 +4324,10 @@
       </c>
       <c r="J68" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K68" s="19" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L68" s="19" t="str">
         <f>"S/S: "&amp;K68</f>
@@ -4339,10 +4339,10 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B69" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C69" t="s">
         <v>9</v>
@@ -4370,10 +4370,10 @@
       </c>
       <c r="J69" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="L69" s="1" t="str">
         <f>"S/S: "&amp;K69</f>
@@ -4382,7 +4382,7 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B70" t="s">
         <v>7</v>
@@ -4413,10 +4413,10 @@
       </c>
       <c r="J70" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L70" s="1" t="str">
         <f>"S/S: "&amp;K70</f>
@@ -4425,10 +4425,10 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B71" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C71" t="s">
         <v>9</v>
@@ -4453,16 +4453,16 @@
       </c>
       <c r="J71" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="L71" s="1"/>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B72" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C72" t="s">
         <v>9</v>
@@ -4487,16 +4487,16 @@
       </c>
       <c r="J72" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="L72" s="1"/>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B73" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C73" t="s">
         <v>9</v>
@@ -4524,10 +4524,10 @@
       </c>
       <c r="J73" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="L73" s="1" t="str">
         <f>"S/S: "&amp;K73</f>
@@ -4536,10 +4536,10 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B74" t="s">
         <v>23</v>
-      </c>
-      <c r="B74" t="s">
-        <v>24</v>
       </c>
       <c r="C74" t="s">
         <v>9</v>
@@ -4568,10 +4568,10 @@
       </c>
       <c r="J74" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="L74" s="1" t="str">
         <f>"S/S: "&amp;K74</f>
@@ -4580,10 +4580,10 @@
     </row>
     <row r="75" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B75" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C75" t="s">
         <v>9</v>
@@ -4612,10 +4612,10 @@
       </c>
       <c r="J75" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K75" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="L75" s="1" t="str">
         <f>"S/S: "&amp;K75</f>
@@ -4625,10 +4625,10 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B76" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C76" t="s">
         <v>9</v>
@@ -4656,10 +4656,10 @@
       </c>
       <c r="J76" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="L76" s="1" t="str">
         <f>"S/S: "&amp;K76</f>
@@ -4668,13 +4668,13 @@
     </row>
     <row r="77" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B77" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C77" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D77">
         <v>1</v>
@@ -4699,10 +4699,10 @@
       </c>
       <c r="J77" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K77" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="M77">
         <v>6</v>
@@ -4710,7 +4710,7 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B78" t="s">
         <v>10</v>
@@ -4741,10 +4741,10 @@
       </c>
       <c r="J78" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L78" s="1" t="str">
         <f>"S/S: "&amp;K78</f>
@@ -4753,10 +4753,10 @@
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B79" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C79" t="s">
         <v>9</v>
@@ -4784,10 +4784,10 @@
       </c>
       <c r="J79" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L79" s="1" t="str">
         <f>"S/S: "&amp;K79</f>
@@ -4796,10 +4796,10 @@
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B80" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C80" t="s">
         <v>9</v>
@@ -4824,15 +4824,15 @@
       </c>
       <c r="J80" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B81" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C81" t="s">
         <v>9</v>
@@ -4860,15 +4860,15 @@
       </c>
       <c r="J81" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>26</v>
+        <v>133</v>
       </c>
       <c r="B82" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C82" t="s">
         <v>9</v>
@@ -4896,10 +4896,10 @@
       </c>
       <c r="J82" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L82" s="1" t="str">
         <f>"S/S: "&amp;K82</f>
@@ -4908,10 +4908,10 @@
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>28</v>
+        <v>134</v>
       </c>
       <c r="B83" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C83" t="s">
         <v>9</v>
@@ -4939,10 +4939,10 @@
       </c>
       <c r="J83" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K83" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L83" s="1" t="str">
         <f>"S/S: "&amp;K83</f>
@@ -4951,10 +4951,10 @@
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B84" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C84" t="s">
         <v>9</v>
@@ -4983,10 +4983,10 @@
       </c>
       <c r="J84" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K84" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="L84" s="1" t="str">
         <f>"S/S: "&amp;K84</f>
@@ -5013,24 +5013,24 @@
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C88" t="s">
         <v>9</v>
       </c>
       <c r="D88">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E88" s="1">
         <f ca="1">dates!$B$3+D88-1</f>
-        <v>44363</v>
+        <v>44364</v>
       </c>
       <c r="G88" s="1">
         <f ca="1">E88+7</f>
-        <v>44370</v>
+        <v>44371</v>
       </c>
       <c r="H88" s="1" t="b">
         <f ca="1">OR(E88&lt;dates!$B$3,E88&gt;dates!$B$4)</f>
@@ -5041,16 +5041,16 @@
       </c>
       <c r="J88" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="L88" s="1"/>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C89" t="s">
         <v>9</v>
@@ -5075,13 +5075,13 @@
       </c>
       <c r="J89" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="L89" s="1"/>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B90" t="s">
         <v>10</v>
@@ -5112,10 +5112,10 @@
       </c>
       <c r="J90" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K90" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="L90" s="1" t="str">
         <f>"S/S: "&amp;K90</f>
@@ -5124,24 +5124,24 @@
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B91" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C91" t="s">
         <v>9</v>
       </c>
       <c r="D91">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="E91" s="1">
         <f ca="1">dates!$B$3+D91-1</f>
-        <v>44363</v>
+        <v>44349</v>
       </c>
       <c r="G91" s="1">
         <f ca="1">E91+7</f>
-        <v>44370</v>
+        <v>44356</v>
       </c>
       <c r="H91" s="1" t="b">
         <f ca="1">OR(E91&lt;dates!$B$3,E91&gt;dates!$B$4)</f>
@@ -5152,16 +5152,16 @@
       </c>
       <c r="J91" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="L91" s="1"/>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B92" t="s">
         <v>91</v>
-      </c>
-      <c r="B92" t="s">
-        <v>94</v>
       </c>
       <c r="C92" t="s">
         <v>9</v>
@@ -5186,16 +5186,16 @@
       </c>
       <c r="J92" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="L92" s="1"/>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B93" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C93" t="s">
         <v>9</v>
@@ -5224,10 +5224,10 @@
       </c>
       <c r="J93" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K93" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L93" s="1" t="str">
         <f>"S/S: "&amp;K93</f>
@@ -5236,10 +5236,10 @@
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B94" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C94" t="s">
         <v>9</v>
@@ -5268,10 +5268,10 @@
       </c>
       <c r="J94" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K94" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L94" s="1" t="str">
         <f>"S/S: "&amp;K94</f>
@@ -5280,7 +5280,7 @@
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B95" t="s">
         <v>7</v>
@@ -5311,10 +5311,10 @@
       </c>
       <c r="J95" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K95" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L95" s="1" t="str">
         <f>"S/S: "&amp;K95</f>
@@ -5323,10 +5323,10 @@
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B96" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C96" t="s">
         <v>9</v>
@@ -5351,16 +5351,16 @@
       </c>
       <c r="J96" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="L96" s="1"/>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B97" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C97" t="s">
         <v>9</v>
@@ -5385,19 +5385,19 @@
       </c>
       <c r="J97" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="L97" s="1"/>
     </row>
     <row r="98" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B98" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C98" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D98">
         <v>1</v>
@@ -5422,10 +5422,10 @@
       </c>
       <c r="J98" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44320.395751157404</v>
+        <v>44320.423062731483</v>
       </c>
       <c r="K98" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="L98" s="1" t="str">
         <f>"S/S: "&amp;K98</f>
@@ -5471,15 +5471,15 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1">
         <f ca="1">EOMONTH(NOW(),0)</f>
@@ -5492,7 +5492,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B3" s="1">
         <f ca="1">EOMONTH(B2,0)+1</f>
@@ -5501,7 +5501,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B4" s="1">
         <f ca="1">EOMONTH(B2,1)</f>
@@ -5510,7 +5510,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B5" s="1">
         <f ca="1">_xlfn.CEILING.MATH((B3+B4)/2,1)</f>
@@ -5519,7 +5519,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B6" s="1">
         <f ca="1">B4+1</f>
@@ -5528,7 +5528,7 @@
     </row>
     <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B7" s="1">
         <f ca="1">DATE(YEAR($B$3),MONTH($B$3),'Which Week'!B8)-WEEKDAY(DATE(YEAR($B$3),MONTH($B$3),'Day of Week'!$B$11))</f>
@@ -5537,7 +5537,7 @@
     </row>
     <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B8" s="1">
         <f ca="1">DATE(YEAR($B$3),MONTH($B$3),'Which Week'!B9)-WEEKDAY(DATE(YEAR($B$3),MONTH($B$3),'Day of Week'!$B$11))</f>
@@ -5546,7 +5546,7 @@
     </row>
     <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B9" s="1">
         <f ca="1">DATE(YEAR($B$3),MONTH($B$3),'Which Week'!B10)-WEEKDAY(DATE(YEAR($B$3),MONTH($B$3),'Day of Week'!$B$11))</f>
@@ -5555,7 +5555,7 @@
     </row>
     <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B10" s="1">
         <f ca="1">DATE(YEAR($B$3),MONTH($B$3),'Which Week'!B11)-WEEKDAY(DATE(YEAR($B$3),MONTH($B$3),'Day of Week'!$B$11))</f>
@@ -5564,7 +5564,7 @@
     </row>
     <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B11" s="1">
         <f ca="1">IF(MONTH(DATE(YEAR($B$3),MONTH($B$3),'Which Week'!B12)-WEEKDAY(DATE(YEAR($B$3),MONTH($B$3),'Day of Week'!$B$11)))=MONTH(B10),DATE(YEAR($B$3),MONTH($B$3),'Which Week'!B12)-WEEKDAY(DATE(YEAR($B$3),MONTH($B$3),'Day of Week'!$B$11)),NA())</f>
@@ -5573,7 +5573,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B12" s="1">
         <f ca="1">DATE(YEAR(B3),1,1)</f>
@@ -5582,7 +5582,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B13">
         <f ca="1">ROUNDUP(MONTH(B3)/3,0)</f>
@@ -5591,7 +5591,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B14" s="1">
         <f ca="1">DATE(YEAR(B12),(3*(B13-1)+1),1)</f>
@@ -5755,7 +5755,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B1" s="21"/>
     </row>
@@ -5773,10 +5773,10 @@
     </row>
     <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5789,7 +5789,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -5797,7 +5797,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -5805,7 +5805,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -5813,7 +5813,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B11">
         <v>4</v>
@@ -5821,7 +5821,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B12">
         <v>5</v>
@@ -5829,7 +5829,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B13">
         <v>6</v>
@@ -5837,7 +5837,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B14">
         <v>7</v>
@@ -5881,7 +5881,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B1" s="11"/>
     </row>
@@ -5899,10 +5899,10 @@
     </row>
     <row r="5" spans="1:6" s="2" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D5"/>
       <c r="F5"/>
@@ -5921,7 +5921,7 @@
     </row>
     <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B8">
         <v>8</v>
@@ -5929,7 +5929,7 @@
     </row>
     <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B9">
         <f>B8+7</f>
@@ -5938,7 +5938,7 @@
     </row>
     <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B10">
         <f>B9+7</f>
@@ -5947,7 +5947,7 @@
     </row>
     <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B11">
         <f>B10+7</f>
@@ -5956,7 +5956,7 @@
     </row>
     <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B12">
         <f>B11+7</f>

</xml_diff>